<commit_message>
project name occ update
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="44">
   <si>
     <t>Execute</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>admin124</t>
+  </si>
+  <si>
+    <t>abcd123</t>
+  </si>
+  <si>
+    <t>testCaseName</t>
   </si>
 </sst>
 </file>
@@ -496,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,13 +667,13 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" customWidth="1"/>
     <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
@@ -723,7 +729,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
@@ -760,10 +766,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,6 +878,90 @@
         <v>40</v>
       </c>
     </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -880,97 +970,101 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" style="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" customWidth="1"/>
+    <col min="5" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Start with Pageobject change and datasheet change
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{92A4402C-A1A1-4CD8-86CD-EE12C2CC9808}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20790" windowHeight="11820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
     <sheet name="IC" sheetId="23" r:id="rId2"/>
-    <sheet name="Login++" sheetId="25" r:id="rId3"/>
-    <sheet name="Russels" sheetId="26" r:id="rId4"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId5"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId6"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId7"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId8"/>
+    <sheet name="AccountCreationUserDetails++" sheetId="31" r:id="rId3"/>
+    <sheet name="Login++" sheetId="25" r:id="rId4"/>
+    <sheet name="Russels" sheetId="26" r:id="rId5"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId6"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId7"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId8"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:H17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="57">
   <si>
     <t>Execute</t>
   </si>
@@ -153,13 +156,52 @@
   </si>
   <si>
     <t>testCaseName</t>
+  </si>
+  <si>
+    <t>Create new customer in IC</t>
+  </si>
+  <si>
+    <t>AccountCreationUserDetails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User_Firstname </t>
+  </si>
+  <si>
+    <t>User_Lastname</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Confirm_password</t>
+  </si>
+  <si>
+    <t>SAID</t>
+  </si>
+  <si>
+    <t>Breno Fernandes</t>
+  </si>
+  <si>
+    <t>Rocha</t>
+  </si>
+  <si>
+    <t>BrenoFernandesRocha@armyspy.com</t>
+  </si>
+  <si>
+    <t>Pass12345</t>
+  </si>
+  <si>
+    <t>9602149977088</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +215,14 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -192,15 +242,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -208,6 +262,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -256,7 +313,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -289,9 +346,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -324,6 +398,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -499,7 +590,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -663,19 +754,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -749,13 +841,27 @@
         <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -765,11 +871,92 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5054DFA-212C-4ABC-86D1-7A882998953C}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D5E82FFD-B67B-4E43-8612-02CD28603562}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,12 +1155,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,8 +1260,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1177,8 +1364,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1281,8 +1468,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1385,8 +1572,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Completed TA8 creating a pull
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -3,26 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FDCF3F-BEAF-4E9D-8698-A737F8CE379F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E66444B-AA1A-46BB-B3AC-948B869F69CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="15285" windowHeight="7875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
     <sheet name="IC" sheetId="23" r:id="rId2"/>
     <sheet name="Login++" sheetId="25" r:id="rId3"/>
-    <sheet name="Russels" sheetId="26" r:id="rId4"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId5"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId6"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId7"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId8"/>
+    <sheet name="Login_magento++" sheetId="31" r:id="rId4"/>
+    <sheet name="Russels" sheetId="26" r:id="rId5"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId6"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId7"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId8"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="53">
   <si>
     <t>Execute</t>
   </si>
@@ -160,6 +161,27 @@
   </si>
   <si>
     <t>iCcartVerification</t>
+  </si>
+  <si>
+    <t>Magento Backend Login</t>
+  </si>
+  <si>
+    <t>Login_magento</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://staging-jdgroup-m23.vaimo.net/T5sjY7drHkyB6Z4n/admin/index/index/key/4cee16108e07c6904ab12f33e9f10b9b1b1fadb7c06faa4c94fbd03a1d1018ff/</t>
+  </si>
+  <si>
+    <t>Access#11</t>
   </si>
 </sst>
 </file>
@@ -208,10 +230,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,14 +579,14 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7265625" customWidth="1"/>
-    <col min="4" max="6" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -586,7 +609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -606,7 +629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -626,7 +649,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -646,7 +669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -666,7 +689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -686,7 +709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -714,24 +737,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -772,7 +795,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -792,7 +815,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -809,7 +832,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -817,10 +840,24 @@
         <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -835,18 +872,18 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -860,7 +897,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -874,7 +911,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -888,7 +925,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -902,7 +939,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -916,7 +953,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -930,7 +967,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -944,7 +981,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -958,7 +995,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -972,7 +1009,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -986,7 +1023,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -1000,7 +1037,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -1014,7 +1051,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -1035,6 +1072,60 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A018AFB-9EBE-4509-AC35-F67BF988EA35}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2">
+        <v>225564</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -1042,18 +1133,18 @@
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="7" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1097,7 +1188,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -1117,7 +1208,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -1139,7 +1230,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1147,17 +1238,17 @@
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1198,7 +1289,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1218,7 +1309,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1243,7 +1334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1251,17 +1342,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1302,7 +1393,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1322,7 +1413,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1347,7 +1438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1355,17 +1446,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1406,7 +1497,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1426,7 +1517,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1451,7 +1542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1459,17 +1550,17 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1510,7 +1601,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1530,7 +1621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
adding magento order search
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -4,40 +4,31 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
     <sheet name="IC" sheetId="23" r:id="rId2"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId3"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId4"/>
-    <sheet name="Russels" sheetId="26" r:id="rId5"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId6"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId7"/>
-    <sheet name="Login++" sheetId="25" r:id="rId8"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId9"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId10"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId11"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId12"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId13"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId3"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId4"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId5"/>
+    <sheet name="Russels" sheetId="26" r:id="rId6"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId7"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId8"/>
+    <sheet name="Login++" sheetId="25" r:id="rId9"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId10"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId11"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId12"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId13"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId14"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="112">
   <si>
     <t>testSuitID</t>
   </si>
@@ -361,6 +352,18 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>OrderStatusSearch</t>
+  </si>
+  <si>
+    <t>Canceled</t>
+  </si>
+  <si>
+    <t>orderStatus</t>
+  </si>
+  <si>
+    <t>productSearchId</t>
   </si>
 </sst>
 </file>
@@ -484,9 +487,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -944,6 +944,84 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1046,7 +1124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1150,7 +1228,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1254,7 +1332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1362,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,7 +1455,8 @@
     <col min="8" max="8" width="18.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="10"/>
@@ -1464,6 +1543,9 @@
       <c r="K2" s="10" t="s">
         <v>106</v>
       </c>
+      <c r="L2" s="10" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -1536,6 +1618,56 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3100000680</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -1627,7 +1759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1684,7 +1816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -1789,7 +1921,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
@@ -1916,7 +2048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1957,7 +2089,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -2161,94 +2293,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -2257,7 +2302,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2406,15 +2451,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2424,7 +2470,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2441,4 +2487,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Flow is after creating a new customer in IC. verify the same details is there in magento backend customer info section and collect the BP number TA 19 is a method call only which will be having the same datasheet so on basis of a flag we have integrated TA19 scenario here in TA15
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE228A0F-F35E-42BB-B570-90F4397F90E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EAD934-EC3E-4103-9BED-C3A5D6E4A397}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="69">
   <si>
     <t>Execute</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>BrenoFernandesSouRochas@armyspy.com</t>
+  </si>
+  <si>
+    <t>VerifyAccountDetailsInMagentoBackend</t>
   </si>
 </sst>
 </file>
@@ -630,14 +633,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7265625" customWidth="1"/>
-    <col min="4" max="6" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -660,7 +663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -680,7 +683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -700,7 +703,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -720,7 +723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -740,7 +743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -760,7 +763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -794,18 +797,18 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" customWidth="1"/>
-    <col min="4" max="5" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -846,7 +849,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -866,7 +869,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -883,7 +886,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -898,7 +901,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
     </row>
   </sheetData>
@@ -909,33 +912,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5054DFA-212C-4ABC-86D1-7A882998953C}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.26953125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -987,8 +992,11 @@
       <c r="Q1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -1037,16 +1045,20 @@
       <c r="Q2" t="s">
         <v>54</v>
       </c>
+      <c r="R2" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{7E4ACF57-A660-45A6-807C-8A457DFE8ACC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 R2" xr:uid="{7E4ACF57-A660-45A6-807C-8A457DFE8ACC}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{3298DDCC-15EA-4EE3-A635-A5C0AB2F4931}">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2 N2 O2 P2 L2 Q2" xr:uid="{C9501321-A586-4737-BFCB-117928C244E7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:Q2" xr:uid="{C9501321-A586-4737-BFCB-117928C244E7}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1066,15 +1078,15 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1088,7 +1100,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1102,7 +1114,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1116,7 +1128,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1130,7 +1142,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1144,7 +1156,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1158,7 +1170,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -1172,7 +1184,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -1186,7 +1198,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -1200,7 +1212,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -1214,7 +1226,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -1228,7 +1240,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -1242,7 +1254,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -1270,18 +1282,18 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="7" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1325,7 +1337,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -1345,7 +1357,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -1375,17 +1387,17 @@
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1426,7 +1438,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1446,7 +1458,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1479,17 +1491,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1530,7 +1542,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1550,7 +1562,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1583,17 +1595,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1634,7 +1646,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1654,7 +1666,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1687,17 +1699,17 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1738,7 +1750,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1758,7 +1770,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
sprint1 Guest user update
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="114">
   <si>
     <t>testSuitID</t>
   </si>
@@ -159,9 +159,6 @@
     <t>specificProduct</t>
   </si>
   <si>
-    <t>PS4 GOD OF WAR</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
     <t>searchbar</t>
   </si>
   <si>
-    <t>playstation</t>
-  </si>
-  <si>
     <t>deliveryPopulation</t>
   </si>
   <si>
@@ -364,6 +358,18 @@
   </si>
   <si>
     <t>productSearchId</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>sumsung</t>
+  </si>
+  <si>
+    <t>Samsung Toner D105L</t>
   </si>
 </sst>
 </file>
@@ -782,7 +788,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,10 +950,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,48 +976,100 @@
         <v>36</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>57</v>
+      <c r="F3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1084,19 +1142,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1104,19 +1162,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1188,19 +1246,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1208,19 +1266,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1292,19 +1350,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1312,19 +1370,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1396,19 +1454,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1416,19 +1474,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1440,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,7 +1515,8 @@
     <col min="10" max="10" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="10"/>
   </cols>
@@ -1467,7 +1526,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>16</v>
@@ -1476,7 +1535,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>17</v>
@@ -1514,10 +1573,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>8</v>
@@ -1529,10 +1588,10 @@
         <v>32</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>33</v>
@@ -1541,10 +1600,10 @@
         <v>34</v>
       </c>
       <c r="K2" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1552,10 +1611,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>9</v>
@@ -1567,10 +1626,10 @@
         <v>32</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>33</v>
@@ -1584,10 +1643,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>9</v>
@@ -1599,10 +1658,10 @@
         <v>32</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>33</v>
@@ -1619,10 +1678,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,10 +1701,10 @@
         <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1659,7 +1718,35 @@
         <v>3100000680</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3100000680</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3100000680</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1672,7 +1759,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E2" sqref="E2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,14 +1799,14 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1730,10 +1817,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1744,13 +1831,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1761,10 +1848,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1785,13 +1872,13 @@
         <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1802,13 +1889,47 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D2" s="1">
         <v>225564</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="1">
+        <v>225564</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="1">
+        <v>225564</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1840,7 +1961,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>16</v>
@@ -1926,7 +2047,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,82 +2073,162 @@
         <v>36</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="J2" s="5">
         <v>2000</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="L2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="H3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" s="5">
+        <v>2000</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="5">
+        <v>2000</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="5" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2042,18 +2243,20 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId2"/>
+    <hyperlink ref="L4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,6 +2284,28 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2113,10 +2338,10 @@
         <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2127,10 +2352,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2141,10 +2366,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2155,10 +2380,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2169,10 +2394,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2183,10 +2408,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2197,10 +2422,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2211,10 +2436,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2225,10 +2450,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2239,10 +2464,10 @@
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2253,10 +2478,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2267,10 +2492,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2281,10 +2506,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TA26 - end to end running code for review. Sprint 2 task
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -1,34 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D4B9E9-91C4-4616-BAF0-6E57AE44573F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
     <sheet name="IC" sheetId="23" r:id="rId2"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId3"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId4"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId5"/>
-    <sheet name="Russels" sheetId="26" r:id="rId6"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId7"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId8"/>
-    <sheet name="Login++" sheetId="25" r:id="rId9"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId10"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId11"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId12"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId13"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId14"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId3"/>
+    <sheet name="CreateaccountBackend++" sheetId="37" r:id="rId4"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId5"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId6"/>
+    <sheet name="Russels" sheetId="26" r:id="rId7"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId8"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId9"/>
+    <sheet name="Login++" sheetId="25" r:id="rId10"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId11"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId12"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId13"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId14"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId15"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="131">
   <si>
     <t>testSuitID</t>
   </si>
@@ -370,12 +371,63 @@
   </si>
   <si>
     <t>Samsung Toner D105L</t>
+  </si>
+  <si>
+    <t>Magento admin register new user</t>
+  </si>
+  <si>
+    <t>Register a new user in magento backend</t>
+  </si>
+  <si>
+    <t>Sourav</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Identitynumber/passport</t>
+  </si>
+  <si>
+    <t>SAID</t>
+  </si>
+  <si>
+    <t>Passport</t>
+  </si>
+  <si>
+    <t>Backend_Fisrtname</t>
+  </si>
+  <si>
+    <t>Backend_Lastname</t>
+  </si>
+  <si>
+    <t>7503226018089</t>
+  </si>
+  <si>
+    <t>CreateaccountBackend</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Main Website</t>
+  </si>
+  <si>
+    <t>DelayforElements</t>
+  </si>
+  <si>
+    <t>TestAutomation5@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -462,7 +514,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -483,6 +535,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -493,6 +547,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -541,7 +598,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -574,9 +631,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -609,6 +683,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -784,7 +875,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -949,7 +1040,211 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1078,8 +1373,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1182,8 +1477,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1286,8 +1581,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1390,8 +1685,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="L14" workbookViewId="0">
@@ -1495,11 +1790,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,8 +1804,7 @@
     <col min="4" max="4" width="8" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
@@ -1579,7 +1873,7 @@
         <v>101</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>31</v>
@@ -1668,6 +1962,29 @@
       </c>
       <c r="J4" s="9" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>6</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1677,7 +1994,213 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="144.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="1">
+        <v>225564</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="1">
+        <v>225564</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="1">
+        <v>225564</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="1">
+        <v>225564</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DABB35B6-A6EE-4ED2-815A-A37DB87FC8AA}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J2">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{A036CF8D-FA9E-46BF-BE93-0EA7D927F869}">
+      <formula1>"SAID,Passport"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{C6AFC271-F731-4F69-AB48-EACC7737CDA1}">
+      <formula1>"Main Website,Incredible Connection"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="TestAutomation2@gmail.com" xr:uid="{16694021-D89F-479B-9BE5-6C2875269D5E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1754,8 +2277,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1846,99 +2369,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="144.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="1">
-        <v>225564</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" s="1">
-        <v>225564</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="1">
-        <v>225564</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2042,8 +2474,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2242,17 +2674,17 @@
     <row r="15" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="L4" r:id="rId3"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2314,211 +2746,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -2527,7 +2764,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2676,16 +2913,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2695,7 +2931,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2712,12 +2948,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TA32-Part 2 _magento replace the local vaiable with sheet parameter points: commited the code in TA32 part2 magneto points needed : parameter the hard code values of expected  2. Before this code we should be calling action to create account which is from leverch        2.1Long magneto then >navigate to all customer  then >filter the email id and> click on edit section then my code will work there after.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6EABB898-EE17-436D-8D06-031809A96671}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20760" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="accountCreation++" sheetId="37" r:id="rId1"/>
-    <sheet name="Suites" sheetId="22" r:id="rId2"/>
-    <sheet name="IC" sheetId="23" r:id="rId3"/>
+    <sheet name="Suites" sheetId="22" r:id="rId1"/>
+    <sheet name="IC" sheetId="23" r:id="rId2"/>
+    <sheet name="accountCreation++" sheetId="37" r:id="rId3"/>
     <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId4"/>
     <sheet name="ProductSearch++" sheetId="33" r:id="rId5"/>
     <sheet name="Login_magento++" sheetId="35" r:id="rId6"/>
@@ -23,12 +24,13 @@
     <sheet name="Sleepmasters" sheetId="29" r:id="rId14"/>
     <sheet name="HiFiCorp" sheetId="30" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="F1:K17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="135">
   <si>
     <t>testSuitID</t>
   </si>
@@ -426,19 +428,19 @@
     <t>Create new customer in IC</t>
   </si>
   <si>
-    <t>accountCreation</t>
-  </si>
-  <si>
-    <t>Verify_Acount_Information</t>
-  </si>
-  <si>
     <t>BrenoFernandesSouRochasf1@armyspy.com</t>
+  </si>
+  <si>
+    <t>Magento_UserInfoVerification</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and verify in magento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -559,6 +561,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -606,7 +611,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -639,9 +644,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -674,6 +696,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -849,10 +888,1054 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView topLeftCell="L14" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="55.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -949,7 +2032,7 @@
         <v>116</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>115</v>
@@ -991,1074 +2074,26 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:Q2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:Q2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 R2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 R2" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView topLeftCell="L14" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="55.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2136,7 +2171,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2228,7 +2263,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2319,7 +2354,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2424,7 +2459,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2623,9 +2658,9 @@
     <row r="15" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="L4" r:id="rId3"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -2633,7 +2668,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2845,21 +2880,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2882,14 +2917,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2897,4 +2924,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
output data sheet and TA10
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -4,31 +4,32 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="accountCreation++" sheetId="37" r:id="rId1"/>
-    <sheet name="Suites" sheetId="22" r:id="rId2"/>
-    <sheet name="IC" sheetId="23" r:id="rId3"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId4"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId5"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId6"/>
-    <sheet name="Russels" sheetId="26" r:id="rId7"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId8"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId9"/>
-    <sheet name="Login++" sheetId="25" r:id="rId10"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId11"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId12"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId13"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId14"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId15"/>
+    <sheet name="IC" sheetId="23" r:id="rId1"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId2"/>
+    <sheet name="accountCreation++" sheetId="37" r:id="rId3"/>
+    <sheet name="Suites" sheetId="22" r:id="rId4"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId5"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId6"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId7"/>
+    <sheet name="Russels" sheetId="26" r:id="rId8"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId9"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId10"/>
+    <sheet name="Login++" sheetId="25" r:id="rId11"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId12"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId13"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId14"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId15"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId16"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="143">
   <si>
     <t>testSuitID</t>
   </si>
@@ -432,7 +433,31 @@
     <t>Verify_Acount_Information</t>
   </si>
   <si>
-    <t>BrenoFernandesSouRochasf1@armyspy.com</t>
+    <t>BrenoFernandesSouRochasf2@armyspy.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create new customer in IC </t>
+  </si>
+  <si>
+    <t>GenerateOrderSAPnumber</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>OrderID</t>
+  </si>
+  <si>
+    <t>OrderSAPnumber</t>
+  </si>
+  <si>
+    <t>totalCounter</t>
+  </si>
+  <si>
+    <t>9109105800081</t>
+  </si>
+  <si>
+    <t>9109105800082</t>
   </si>
 </sst>
 </file>
@@ -850,10 +875,1015 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="55.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView topLeftCell="L14" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,762 +2039,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView topLeftCell="L14" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,140 +2204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="55.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -2135,12 +2282,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2227,12 +2374,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C8:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,7 +2465,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -2423,12 +2570,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A5" sqref="A5:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2566,7 +2713,7 @@
         <v>80</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>81</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2607,20 +2754,9 @@
         <v>80</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1"/>
@@ -2629,69 +2765,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2892,9 +2965,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TA32 PArt 2 Magento validation part
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6EABB898-EE17-436D-8D06-031809A96671}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98955450-3166-4B42-9314-5B9C6ECF4847}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="20760" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="15285" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
@@ -25,12 +25,11 @@
     <sheet name="HiFiCorp" sheetId="30" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="F1:K17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="139">
   <si>
     <t>testSuitID</t>
   </si>
@@ -377,21 +376,12 @@
     <t>ID</t>
   </si>
   <si>
-    <t>James12Runs</t>
-  </si>
-  <si>
     <t>Jones</t>
   </si>
   <si>
     <t>Brian</t>
   </si>
   <si>
-    <t>VerifyAccountDetailsInMagentoBackend</t>
-  </si>
-  <si>
-    <t>verifyAccount</t>
-  </si>
-  <si>
     <t>validateIncorrectID</t>
   </si>
   <si>
@@ -428,13 +418,34 @@
     <t>Create new customer in IC</t>
   </si>
   <si>
-    <t>BrenoFernandesSouRochasf1@armyspy.com</t>
-  </si>
-  <si>
     <t>Magento_UserInfoVerification</t>
   </si>
   <si>
-    <t>Create new customer in IC and verify in magento</t>
+    <t>TestCaseName</t>
+  </si>
+  <si>
+    <t>vatNumberFlag</t>
+  </si>
+  <si>
+    <t>WebSite</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate VAT Number</t>
+  </si>
+  <si>
+    <t>BrenoFernandesMalingaPatrick@armyspy.com</t>
+  </si>
+  <si>
+    <t>Password2</t>
+  </si>
+  <si>
+    <t>Incredible Connection</t>
+  </si>
+  <si>
+    <t>Create new customer in IC using VAT and verify in magento</t>
+  </si>
+  <si>
+    <t>accountCreation</t>
   </si>
 </sst>
 </file>
@@ -527,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -548,7 +559,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1806,8 +1816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,7 +1825,9 @@
     <col min="1" max="1" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="55.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
@@ -1913,16 +1925,25 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>133</v>
+        <v>101</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1933,36 +1954,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="48.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1970,31 +1992,31 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>124</v>
@@ -2017,8 +2039,11 @@
       <c r="R1" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -2026,37 +2051,40 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>132</v>
+      <c r="E2" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>115</v>
+        <v>134</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="1">
+        <v>2222224</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>112</v>
@@ -2065,27 +2093,33 @@
         <v>112</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:Q2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{16388FA5-1B70-4343-AAEB-820658200196}">
+      <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:S2 I2" xr:uid="{D45FDEF1-D73A-426C-82C7-A8256A573A08}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{5F2C8A28-8880-4A13-808B-DDF757AD57B0}">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 R2" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{FE3A07B9-D2E5-4986-BB90-04B4B9832BD4}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{55C1AF6E-D58F-4A99-9595-B4436AC772B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -2097,7 +2131,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2267,7 +2301,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2731,6 +2765,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2879,25 +2931,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2914,22 +2966,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TA32 review and code updates
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
     <sheet name="IC" sheetId="23" r:id="rId2"/>
     <sheet name="accountCreation++" sheetId="39" r:id="rId3"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId4"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId5"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId6"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId7"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId4"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId5"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId6"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId7"/>
     <sheet name="Russels" sheetId="26" r:id="rId8"/>
     <sheet name="deliveryPopulation++" sheetId="34" r:id="rId9"/>
     <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId10"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="151">
   <si>
     <t>testSuitID</t>
   </si>
@@ -295,18 +295,12 @@
     <t>8</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>https://staging-jdgroup-m23.vaimo.net/T5sjY7drHkyB6Z4n/admin/index/index/key/4cee16108e07c6904ab12f33e9f10b9b1b1fadb7c06faa4c94fbd03a1d1018ff/</t>
-  </si>
-  <si>
     <t>Access#11</t>
   </si>
   <si>
@@ -485,13 +479,16 @@
   </si>
   <si>
     <t>GENERATED EMAIL</t>
+  </si>
+  <si>
+    <t>Magento_UserInfoVerification</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,6 +537,13 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -583,7 +587,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -608,6 +612,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1437,12 +1442,12 @@
         <v>54</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1">
       <c r="A2" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1468,7 +1473,7 @@
     </row>
     <row r="3" spans="1:9" s="4" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -1494,7 +1499,7 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1">
       <c r="A4" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -1944,8 +1949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1953,7 +1958,8 @@
     <col min="1" max="1" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="55.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
@@ -1970,7 +1976,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>16</v>
@@ -1979,7 +1985,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>17</v>
@@ -2017,10 +2023,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -2041,13 +2047,13 @@
         <v>33</v>
       </c>
       <c r="K2" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>103</v>
-      </c>
       <c r="M2" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1">
@@ -2055,19 +2061,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1">
@@ -2075,16 +2081,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="1" customFormat="1">
@@ -2092,16 +2104,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="1" customFormat="1">
@@ -2109,16 +2127,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="1" customFormat="1">
@@ -2126,16 +2150,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="1" customFormat="1">
@@ -2143,32 +2173,38 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G4">
+  <conditionalFormatting sqref="H4">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
+  <conditionalFormatting sqref="H5">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
+  <conditionalFormatting sqref="H6">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
+  <conditionalFormatting sqref="H7">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
+  <conditionalFormatting sqref="H8">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2180,8 +2216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F6"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2216,55 +2252,55 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>71</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -2275,55 +2311,55 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J2" s="1">
         <v>2222224</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="N2" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>113</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -2334,55 +2370,55 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J3" s="1">
         <v>2222225</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="N3" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -2393,55 +2429,55 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J4" s="1">
         <v>2222226</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N4" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>113</v>
-      </c>
       <c r="O4" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2452,55 +2488,55 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J5" s="1">
         <v>2222227</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -2511,55 +2547,55 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J6" s="1">
         <v>2222228</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="N6" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2584,10 +2620,157 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>225564</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>225564</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>225564</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>225564</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>225564</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>225564</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>225564</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>225564</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2606,13 +2789,13 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2634,7 +2817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -2659,10 +2842,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2676,7 +2859,7 @@
         <v>3100000680</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2690,7 +2873,7 @@
         <v>3100000680</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2704,7 +2887,7 @@
         <v>3100000680</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2712,7 +2895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -2761,10 +2944,10 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1">
@@ -2775,10 +2958,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1">
@@ -2789,109 +2972,18 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C8:C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="144.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="1">
-        <v>225564</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="1">
-        <v>225564</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="1">
-        <v>225564</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3066,7 +3158,7 @@
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1">
       <c r="A2" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -3107,7 +3199,7 @@
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1">
       <c r="A3" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -3143,12 +3235,12 @@
         <v>80</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -3184,7 +3276,7 @@
         <v>80</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new ICUpdate customer updates
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C99A2EA-002D-4B2B-AB5C-5AAD73B46AE2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA446C3-0622-4CFC-9D17-D3F9401A8226}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ic_login++" sheetId="38" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="147">
   <si>
     <t>testSuitID</t>
   </si>
@@ -404,6 +404,9 @@
     <t>Password@123</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Northern Cape</t>
   </si>
   <si>
@@ -416,43 +419,58 @@
     <t>billing_streetAddress</t>
   </si>
   <si>
-    <t>billing_buildingDetails</t>
-  </si>
-  <si>
-    <t>billing_province</t>
-  </si>
-  <si>
-    <t>billing_provinceName</t>
-  </si>
-  <si>
-    <t>billing_city</t>
-  </si>
-  <si>
-    <t>billing_suburb</t>
-  </si>
-  <si>
-    <t>billing_postalCode</t>
-  </si>
-  <si>
     <t>shipping_streetAddress</t>
   </si>
   <si>
-    <t>shipping_buildingDetails</t>
-  </si>
-  <si>
-    <t>shipping_province</t>
-  </si>
-  <si>
-    <t>shipping_provinceName</t>
-  </si>
-  <si>
-    <t>shipping_city</t>
-  </si>
-  <si>
-    <t>shipping_suburb</t>
-  </si>
-  <si>
-    <t>shipping_postalCode</t>
+    <t>firstName_output</t>
+  </si>
+  <si>
+    <t>lastName_output</t>
+  </si>
+  <si>
+    <t>taxVat_output</t>
+  </si>
+  <si>
+    <t>passWord_output</t>
+  </si>
+  <si>
+    <t>email_output</t>
+  </si>
+  <si>
+    <t>shipping_streetAddress_Output</t>
+  </si>
+  <si>
+    <t>billing_streetAddress_output</t>
+  </si>
+  <si>
+    <t>billing_buildingDetails_output</t>
+  </si>
+  <si>
+    <t>billing_provinceName_output</t>
+  </si>
+  <si>
+    <t>billing_city_output</t>
+  </si>
+  <si>
+    <t>billing_suburb_output</t>
+  </si>
+  <si>
+    <t>billing_postalCode_output</t>
+  </si>
+  <si>
+    <t>shipping_buildingDetails_output</t>
+  </si>
+  <si>
+    <t>shipping_city_output</t>
+  </si>
+  <si>
+    <t>shipping_suburb_output</t>
+  </si>
+  <si>
+    <t>shipping_postalCode_output</t>
+  </si>
+  <si>
+    <t>shipping_provinceName_output</t>
   </si>
 </sst>
 </file>
@@ -2189,7 +2207,7 @@
         <v>121</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
@@ -2214,7 +2232,7 @@
         <v>121</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -2239,7 +2257,7 @@
         <v>121</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -2252,36 +2270,41 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24F118F-C7C9-45C1-9C92-8C58E2F935F9}">
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.54296875" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.453125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -2291,68 +2314,83 @@
       <c r="C1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" t="s">
         <v>114</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" t="s">
         <v>117</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K1" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>128</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="P1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="R1" t="s">
+        <v>139</v>
+      </c>
+      <c r="S1" t="s">
+        <v>140</v>
+      </c>
+      <c r="T1" t="s">
+        <v>141</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="M1" t="s">
-        <v>131</v>
-      </c>
-      <c r="N1" t="s">
-        <v>132</v>
-      </c>
-      <c r="O1" t="s">
-        <v>133</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="X1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4</v>
       </c>
@@ -2360,70 +2398,48 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
+        <v>126</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+    </row>
+    <row r="3" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>5</v>
       </c>
@@ -2433,68 +2449,38 @@
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>6</v>
       </c>
@@ -2504,68 +2490,38 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="I4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>7</v>
       </c>
@@ -2575,68 +2531,46 @@
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
       <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="I5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="K5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="P5" s="1"/>
       <c r="Q5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>124</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
       <c r="U5" s="1" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>8</v>
       </c>
@@ -2646,68 +2580,46 @@
       <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="K6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>124</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
       <c r="U6" s="1" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>9</v>
       </c>
@@ -2717,68 +2629,46 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>124</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
       <c r="U7" s="1" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>10</v>
       </c>
@@ -2788,68 +2678,46 @@
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="I8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J8" t="s">
-        <v>8</v>
-      </c>
       <c r="K8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>124</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
       <c r="U8" s="1" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>11</v>
       </c>
@@ -2859,68 +2727,46 @@
       <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="I9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="K9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="P9" s="1"/>
       <c r="Q9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>124</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
       <c r="U9" s="1" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>12</v>
       </c>
@@ -2930,68 +2776,46 @@
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="I10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="K10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M10" t="s">
-        <v>8</v>
+        <v>126</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="P10" s="1"/>
       <c r="Q10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>124</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
       <c r="U10" s="1" t="s">
-        <v>8</v>
+        <v>126</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>13</v>
       </c>
@@ -3001,68 +2825,46 @@
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="I11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="K11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N11" t="s">
-        <v>8</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="N11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P11" s="1"/>
       <c r="Q11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>124</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
       <c r="U11" s="1" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>14</v>
       </c>
@@ -3072,83 +2874,59 @@
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="I12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O12" t="s">
-        <v>8</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="P12" s="1"/>
       <c r="Q12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>124</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
       <c r="U12" s="1" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2 S2" xr:uid="{061E9B0E-9193-4026-9902-114AB038C6A6}">
-      <formula1>"Yes, No"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q14 Y3:Y13" xr:uid="{F2D5C2CC-A1AA-447E-8FFC-4E5E2A136C9F}">
+      <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L14 T3:T13" xr:uid="{F2D5C2CC-A1AA-447E-8FFC-4E5E2A136C9F}">
-      <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576 M2:M13 E2:E12 G2:G12 I2:I12 K2:K12 N2:O12 U2:W12" xr:uid="{314C0E9B-B7EF-4634-ADC0-01BA1749AC3F}">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update-Add to cart from excel list done.
Bug->On some iterations, error occurs.
Validation has NOT been added.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -1,35 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A60C9B3-2485-4F3E-AFD0-C9721DD73AA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
     <sheet name="IC" sheetId="23" r:id="rId2"/>
-    <sheet name="accountCreation++" sheetId="39" r:id="rId3"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId4"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId5"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId6"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId7"/>
-    <sheet name="Russels" sheetId="26" r:id="rId8"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId9"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId10"/>
-    <sheet name="Login++" sheetId="25" r:id="rId11"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId12"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId13"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId14"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId15"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId16"/>
+    <sheet name="ProductSearch++" sheetId="42" r:id="rId3"/>
+    <sheet name="CategorySheet" sheetId="41" r:id="rId4"/>
+    <sheet name="accountCreation++" sheetId="39" r:id="rId5"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId6"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId7"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId8"/>
+    <sheet name="Russels" sheetId="26" r:id="rId9"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId10"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId11"/>
+    <sheet name="Login++" sheetId="25" r:id="rId12"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId13"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId14"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId15"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId16"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId17"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId18"/>
+  </externalReferences>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="179">
   <si>
     <t>testSuitID</t>
   </si>
@@ -148,12 +153,6 @@
     <t>typeSearch</t>
   </si>
   <si>
-    <t>categorySearch</t>
-  </si>
-  <si>
-    <t>productsToSearch</t>
-  </si>
-  <si>
     <t>specificProduct</t>
   </si>
   <si>
@@ -214,9 +213,6 @@
     <t>iCcartVerification</t>
   </si>
   <si>
-    <t>searchbar</t>
-  </si>
-  <si>
     <t>deliveryPopulation</t>
   </si>
   <si>
@@ -304,21 +300,6 @@
     <t>Access#11</t>
   </si>
   <si>
-    <t>general</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>Photography </t>
-  </si>
-  <si>
-    <t>CANON DIGITAL CAM IXUS 185 BLACK</t>
-  </si>
-  <si>
-    <t>OFA SAMSUNG REMOTE URC1910</t>
-  </si>
-  <si>
     <t>Create Sales order with guest user- using product search bar</t>
   </si>
   <si>
@@ -352,12 +333,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>sumsung</t>
-  </si>
-  <si>
-    <t>Samsung Toner D105L</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -482,12 +457,127 @@
   </si>
   <si>
     <t>Magento_UserInfoVerification</t>
+  </si>
+  <si>
+    <t>Computer Accessories</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>All Products</t>
+  </si>
+  <si>
+    <t>SearchUsingSearchBar</t>
+  </si>
+  <si>
+    <t>Computers Notebooks &amp; Tablet's</t>
+  </si>
+  <si>
+    <t>Cellphones &amp; Accessories</t>
+  </si>
+  <si>
+    <t>Gaming, Gadgets &amp; Wearables</t>
+  </si>
+  <si>
+    <t>Printing, Scanners &amp; Ink</t>
+  </si>
+  <si>
+    <t>TVs, Displays &amp; Audio</t>
+  </si>
+  <si>
+    <t>Fitness &amp; Wearables</t>
+  </si>
+  <si>
+    <t>Office Solutions</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>Photography</t>
+  </si>
+  <si>
+    <t>Home Security</t>
+  </si>
+  <si>
+    <t>Office Appliances</t>
+  </si>
+  <si>
+    <t>Gift Voucher</t>
+  </si>
+  <si>
+    <t>Downloads &amp; Top Ups</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B40</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B41</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B42</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B43</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B44</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B45</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B46</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B47</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B48</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B49</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B50</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B51</t>
+  </si>
+  <si>
+    <t>searchProduct</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B36</t>
+  </si>
+  <si>
+    <t>JBL EARPHONE T110 BLUE#Xbox One Stealth 600 Gaming Headsets#APPLE TV 4K 64GB MP7P2SOA#OFA 8 In 1 Universal Remote URC1280</t>
+  </si>
+  <si>
+    <t>2#1#2#4</t>
+  </si>
+  <si>
+    <t>Snug Car Juice 3.4A Charger Light Cable - Black#Snug 8000mAh Powerbank LCD Quick Charge Black#SNUG MFI LIGHTING CABLE 1.2M-WHITE</t>
+  </si>
+  <si>
+    <t>2#3#1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+SNUG MFI LIGHTING CABLE 2M-WHITE#Solo Urban Metro Universal Fit 5.5-8.5-inch Tablet Case - Bl#Body Glove Apple iPad 9.7-inch (2017) Smartsuit-Black</t>
+  </si>
+  <si>
+    <t>3#1#2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -587,7 +677,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -613,12 +703,28 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -675,8 +781,42 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Suites"/>
+      <sheetName val="IC"/>
+      <sheetName val="ProductSearch++"/>
+      <sheetName val="CategorySheet"/>
+      <sheetName val="Login++"/>
+      <sheetName val="Russels"/>
+      <sheetName val="Bradlows"/>
+      <sheetName val="Rochester"/>
+      <sheetName val="Sleepmasters"/>
+      <sheetName val="HiFiCorp"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -722,7 +862,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -755,9 +895,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -790,6 +947,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -965,18 +1139,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" customWidth="1"/>
+    <col min="4" max="6" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1130,17 +1304,215 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="5" customFormat="1">
+      <c r="A1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="5" customFormat="1">
+      <c r="A2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="5">
+        <v>2000</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="5" customFormat="1">
+      <c r="A3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="5">
+        <v>2000</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="5" customFormat="1">
+      <c r="A4" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" s="5">
+        <v>2000</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1192,20 +1564,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
@@ -1216,10 +1588,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1230,10 +1602,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1244,10 +1616,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1">
@@ -1258,10 +1630,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1">
@@ -1272,10 +1644,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1">
@@ -1286,10 +1658,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1">
@@ -1300,10 +1672,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1">
@@ -1314,10 +1686,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1">
@@ -1328,10 +1700,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1">
@@ -1342,10 +1714,10 @@
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1">
@@ -1356,10 +1728,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1">
@@ -1370,10 +1742,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1">
@@ -1384,10 +1756,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1396,24 +1768,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
     <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
@@ -1424,103 +1796,103 @@
         <v>35</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1">
       <c r="A2" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="4" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1">
       <c r="A4" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1529,22 +1901,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -1593,19 +1965,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1">
@@ -1613,19 +1985,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1633,22 +2005,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -1697,19 +2069,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1">
@@ -1717,19 +2089,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1737,22 +2109,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -1801,19 +2173,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1">
@@ -1821,19 +2193,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1841,22 +2213,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="L14" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -1905,19 +2277,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1">
@@ -1925,19 +2297,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1946,29 +2318,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="55.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="10.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="55.26953125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="25.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.1796875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -1976,7 +2348,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>16</v>
@@ -1985,7 +2357,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>17</v>
@@ -2023,10 +2395,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -2035,10 +2407,10 @@
         <v>31</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>32</v>
@@ -2047,13 +2419,13 @@
         <v>33</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1">
@@ -2061,19 +2433,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1">
@@ -2081,22 +2453,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="1" customFormat="1">
@@ -2104,22 +2476,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="1" customFormat="1">
@@ -2127,22 +2499,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="1" customFormat="1">
@@ -2150,22 +2522,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="1" customFormat="1">
@@ -2173,38 +2545,298 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="1" customFormat="1">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>150</v>
+      <c r="B9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="1">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>15</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>16</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>17</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
+  <conditionalFormatting sqref="H6">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
+  <conditionalFormatting sqref="H7">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="H8">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
+  <conditionalFormatting sqref="H9">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2213,35 +2845,500 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF5BF71-5B31-4961-B4EF-06A87F6CBCD0}">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.90625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="107.54296875" style="1" customWidth="1"/>
+    <col min="5" max="166" width="8.7265625" style="1"/>
+    <col min="167" max="167" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="168" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="29">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.5">
+      <c r="A5" s="1">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="D19" s="17"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="D20" s="17"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="D21" s="17"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="D22" s="17"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="D24" s="17"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="D25" s="17"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="D27" s="17"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="D28" s="17"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="D29" s="17"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="D31" s="17"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="D32" s="17"/>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="17"/>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" s="17"/>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="D36" s="17"/>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="D37" s="17"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C86:C95" xr:uid="{C677DE07-1970-4D17-801D-FAE9D2FD8E49}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BC3C10AA-6546-417D-8A7D-7C7509DB02FC}">
+          <x14:formula1>
+            <xm:f>'C:\Users\37601\git\JD_IC_TestAutomation\src\test\resources\data\[jdgroupTA3.xlsx]CategorySheet'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>C44:C85</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E4A47391-0A66-435B-8A33-AA5ABAE1119D}">
+          <x14:formula1>
+            <xm:f>CategorySheet!$A$1:$A$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C43</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0AA1275-73C2-40A6-AA60-ADC93C74B2A1}">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="28.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -2252,55 +3349,55 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -2311,55 +3408,55 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="J2" s="1">
         <v>2222224</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -2370,55 +3467,55 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="J3" s="1">
         <v>2222225</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -2429,55 +3526,55 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="J4" s="1">
         <v>2222226</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2488,55 +3585,55 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="J5" s="1">
         <v>2222227</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -2547,69 +3644,69 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>149</v>
-      </c>
       <c r="G6" s="14" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="J6" s="1">
         <v>2222228</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K6" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:S6 I2:I6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:S6 I2:I6" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M6" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L6" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2618,20 +3715,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2642,10 +3739,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2659,7 +3756,7 @@
         <v>225564</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2673,7 +3770,7 @@
         <v>225564</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2687,7 +3784,7 @@
         <v>225564</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2701,7 +3798,7 @@
         <v>225564</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2715,7 +3812,7 @@
         <v>225564</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2729,7 +3826,7 @@
         <v>225564</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2743,7 +3840,7 @@
         <v>225564</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2757,7 +3854,7 @@
         <v>225564</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2765,20 +3862,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2789,13 +3886,13 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2817,21 +3914,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2842,10 +3939,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2859,7 +3956,7 @@
         <v>3100000680</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2873,7 +3970,7 @@
         <v>3100000680</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2887,7 +3984,7 @@
         <v>3100000680</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2895,115 +3992,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
@@ -3011,7 +4016,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>16</v>
@@ -3092,214 +4097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1">
-      <c r="A1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="5" customFormat="1">
-      <c r="A2" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" s="5">
-        <v>2000</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="5" customFormat="1">
-      <c r="A3" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J3" s="5">
-        <v>2000</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="5" customFormat="1">
-      <c r="A4" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J4" s="5">
-        <v>2000</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="L4" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3448,6 +4246,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3458,14 +4265,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3480,6 +4279,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Editing users on IC
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA446C3-0622-4CFC-9D17-D3F9401A8226}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4C1482-C82E-424E-8AB8-05A2E24B37DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ic_login++" sheetId="38" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="155">
   <si>
     <t>testSuitID</t>
   </si>
@@ -398,9 +398,6 @@
     <t>ic_login</t>
   </si>
   <si>
-    <t>OmegaRWilliams@dayrep.com</t>
-  </si>
-  <si>
     <t>Password@123</t>
   </si>
   <si>
@@ -471,6 +468,33 @@
   </si>
   <si>
     <t>shipping_provinceName_output</t>
+  </si>
+  <si>
+    <t>LauraPLittle@teleworm.us</t>
+  </si>
+  <si>
+    <t>user update in IC  All updates</t>
+  </si>
+  <si>
+    <t>user update in IC first name</t>
+  </si>
+  <si>
+    <t>user update in IC last name</t>
+  </si>
+  <si>
+    <t>user update in IC vat/tax</t>
+  </si>
+  <si>
+    <t>user update in IC  email</t>
+  </si>
+  <si>
+    <t>user update in IC password</t>
+  </si>
+  <si>
+    <t>user update in IC  billing address</t>
+  </si>
+  <si>
+    <t>user update in IC  shipping address</t>
   </si>
 </sst>
 </file>
@@ -930,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C38EDD-367C-4E31-8605-DA53A3520421}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="A3" sqref="A3:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -973,11 +997,11 @@
       <c r="C2" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -990,11 +1014,11 @@
       <c r="C3" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1007,11 +1031,130 @@
       <c r="C4" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>123</v>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1019,6 +1162,22 @@
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{60B7B409-2B1E-458F-B2D4-8CE4C1A5822E}"/>
     <hyperlink ref="E4" r:id="rId2" xr:uid="{7438EFE0-9A20-4DEC-AC32-39302C85C190}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{B29A9A4B-201C-4689-9F53-59952D54A63D}"/>
+    <hyperlink ref="D3:D4" r:id="rId4" display="LauraPLittle@teleworm.us" xr:uid="{E53240CB-CE3D-4746-83EB-A2E2B7467F29}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{BD89B053-9040-4E85-A582-426A130DCA15}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{1FDFAE01-216F-41E4-9D91-726D32089790}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{6D264D12-BBA8-42A0-AC4A-B73571AEAC03}"/>
+    <hyperlink ref="D6" r:id="rId8" xr:uid="{99A4B4D1-F399-4D5F-9FE0-B48086A536FE}"/>
+    <hyperlink ref="E7" r:id="rId9" xr:uid="{57289225-B645-4113-9E0C-5972FAB6C03B}"/>
+    <hyperlink ref="D7" r:id="rId10" xr:uid="{5B918F83-769A-4DA6-9C09-7BF6D5DD532C}"/>
+    <hyperlink ref="E8" r:id="rId11" xr:uid="{13B44ADB-3DAA-45FE-B09B-8CCBD329D0E9}"/>
+    <hyperlink ref="D8" r:id="rId12" xr:uid="{7480715A-2DA0-415A-AACF-E73BE90299D7}"/>
+    <hyperlink ref="E9" r:id="rId13" xr:uid="{878FC2A2-4DEE-45E0-9728-186FE81103D8}"/>
+    <hyperlink ref="D9" r:id="rId14" xr:uid="{3B302652-81FF-45E4-B61F-DBD5E3EB12F9}"/>
+    <hyperlink ref="E10" r:id="rId15" xr:uid="{15797308-C950-4BC4-BE0A-A4E4E8564226}"/>
+    <hyperlink ref="D10" r:id="rId16" xr:uid="{5433F0B0-FB62-4095-9D39-6F5ECA828BA5}"/>
+    <hyperlink ref="E11" r:id="rId17" xr:uid="{5B67D7C1-D8BF-4EF9-88BD-809FF78F7B0F}"/>
+    <hyperlink ref="D11" r:id="rId18" xr:uid="{B1D19CCB-6CFE-469D-A039-566E086C6F85}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2004,10 +2163,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2195,10 +2354,10 @@
         <v>116</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>31</v>
@@ -2207,7 +2366,7 @@
         <v>121</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
@@ -2220,10 +2379,10 @@
         <v>116</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>31</v>
@@ -2232,7 +2391,7 @@
         <v>121</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -2245,7 +2404,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>8</v>
@@ -2257,10 +2416,133 @@
         <v>121</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2272,8 +2554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24F118F-C7C9-45C1-9C92-8C58E2F935F9}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2315,79 +2597,79 @@
         <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E1" t="s">
         <v>114</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G1" t="s">
         <v>117</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I1" t="s">
         <v>73</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K1" t="s">
         <v>118</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>119</v>
       </c>
       <c r="N1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="P1" t="s">
         <v>136</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" t="s">
         <v>138</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>139</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>140</v>
-      </c>
-      <c r="T1" t="s">
-        <v>141</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>120</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.35">
@@ -2398,38 +2680,38 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1" t="s">
@@ -2447,7 +2729,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
@@ -2459,25 +2741,25 @@
         <v>9</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="U3" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="V3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -2491,7 +2773,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
@@ -2500,25 +2782,25 @@
         <v>9</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="V4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
@@ -2535,36 +2817,36 @@
         <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="X5" s="1"/>
       <c r="Y5" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
@@ -2587,33 +2869,33 @@
         <v>9</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="X6" s="1"/>
       <c r="Y6" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
@@ -2639,30 +2921,30 @@
         <v>9</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="X7" s="1"/>
       <c r="Y7" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
@@ -2688,30 +2970,30 @@
         <v>9</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
@@ -2737,30 +3019,30 @@
         <v>9</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="X9" s="1"/>
       <c r="Y9" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
@@ -2786,30 +3068,30 @@
         <v>9</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="X10" s="1"/>
       <c r="Y10" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
@@ -2835,30 +3117,30 @@
         <v>9</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
@@ -2884,30 +3166,30 @@
         <v>9</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="X12" s="1"/>
       <c r="Y12" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
@@ -3519,15 +3801,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3676,6 +3949,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
@@ -3685,16 +3967,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3711,4 +3983,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update user on the magento and validate the front data with the
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -1,36 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8A2FBE-A6C8-4194-928C-C8C5C4AF0F62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
     <sheet name="IC" sheetId="23" r:id="rId2"/>
-    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId3"/>
-    <sheet name="accountCreation++" sheetId="39" r:id="rId4"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId5"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId6"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId7"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId8"/>
-    <sheet name="Russels" sheetId="26" r:id="rId9"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId10"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId11"/>
-    <sheet name="Login++" sheetId="25" r:id="rId12"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId13"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId14"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId15"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId16"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId17"/>
+    <sheet name="adminUserUpdate++" sheetId="43" r:id="rId3"/>
+    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId4"/>
+    <sheet name="accountCreation++" sheetId="39" r:id="rId5"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId6"/>
+    <sheet name="customerValidationUpdates++" sheetId="42" r:id="rId7"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId8"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId9"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId10"/>
+    <sheet name="Russels" sheetId="26" r:id="rId11"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId12"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId13"/>
+    <sheet name="Login++" sheetId="25" r:id="rId14"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId15"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId16"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId17"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId18"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId19"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="199">
   <si>
     <t>testSuitID</t>
   </si>
@@ -531,13 +534,109 @@
   </si>
   <si>
     <t>BPnumber</t>
+  </si>
+  <si>
+    <t>adminFirstName_output</t>
+  </si>
+  <si>
+    <t>adminLastName_output</t>
+  </si>
+  <si>
+    <t>taxVat</t>
+  </si>
+  <si>
+    <t>adminTaxVat_output</t>
+  </si>
+  <si>
+    <t>adminEmail_output</t>
+  </si>
+  <si>
+    <t>billingAddress</t>
+  </si>
+  <si>
+    <t>billing_streetAddress</t>
+  </si>
+  <si>
+    <t>adminBilling_streetAddress_output</t>
+  </si>
+  <si>
+    <t>billing_buildingDetails_output</t>
+  </si>
+  <si>
+    <t>billing_provinceName_output</t>
+  </si>
+  <si>
+    <t>billing_city_output</t>
+  </si>
+  <si>
+    <t>billing_suburb_output</t>
+  </si>
+  <si>
+    <t>billing_postalCode_output</t>
+  </si>
+  <si>
+    <t>shippingAddress</t>
+  </si>
+  <si>
+    <t>shipping_buildingDetails_output</t>
+  </si>
+  <si>
+    <t>shipping_provinceName_output</t>
+  </si>
+  <si>
+    <t>shipping_city_output</t>
+  </si>
+  <si>
+    <t>shipping_suburb_output</t>
+  </si>
+  <si>
+    <t>shipping_postalCode_output</t>
+  </si>
+  <si>
+    <t>Northern Cape</t>
+  </si>
+  <si>
+    <t>adminUserUpdate</t>
+  </si>
+  <si>
+    <t>Update customer information on Magento</t>
+  </si>
+  <si>
+    <t>Bongi</t>
+  </si>
+  <si>
+    <t>shipping_streetAddress</t>
+  </si>
+  <si>
+    <t>LauraPLittle@teleworm.us</t>
+  </si>
+  <si>
+    <t>adminShipping_streetAddress_Output</t>
+  </si>
+  <si>
+    <t>Update customer information Mangento All update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updating customer first name on Magento </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updating customer last name on Magento  </t>
+  </si>
+  <si>
+    <t>Updating customer's email on Magento</t>
+  </si>
+  <si>
+    <t>Updating customer's billing address on Magento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updating customers shipping on Magento </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -589,6 +688,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -725,6 +830,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -772,7 +880,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -805,9 +913,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -840,6 +965,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1015,18 +1157,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" customWidth="1"/>
+    <col min="4" max="6" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1180,26 +1322,223 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" customWidth="1"/>
+    <col min="5" max="7" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1">
+      <c r="A2" s="1">
+        <v>99</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>100</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="5" customFormat="1">
@@ -1368,27 +1707,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="L4" r:id="rId3"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1440,20 +1779,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
@@ -1644,24 +1983,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
     <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
@@ -1777,22 +2116,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -1881,22 +2220,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -1985,22 +2324,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -2089,22 +2428,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="L14" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -2194,29 +2533,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="55.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="10.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="55.26953125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="25.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.1796875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2450,7 +2789,7 @@
         <v>163</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>164</v>
@@ -2460,6 +2799,144 @@
       </c>
       <c r="G9" s="10" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="17">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="17">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="17">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="17">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="17">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="17">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2484,27 +2961,369 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C59FE87-E0B0-46B2-B1F3-245D04193D71}">
+  <dimension ref="A1:Z7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L1" t="s">
+        <v>173</v>
+      </c>
+      <c r="M1" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" t="s">
+        <v>175</v>
+      </c>
+      <c r="O1" t="s">
+        <v>176</v>
+      </c>
+      <c r="P1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>178</v>
+      </c>
+      <c r="R1" t="s">
+        <v>179</v>
+      </c>
+      <c r="S1" t="s">
+        <v>180</v>
+      </c>
+      <c r="T1" t="s">
+        <v>190</v>
+      </c>
+      <c r="U1" t="s">
+        <v>192</v>
+      </c>
+      <c r="V1" t="s">
+        <v>181</v>
+      </c>
+      <c r="W1" t="s">
+        <v>182</v>
+      </c>
+      <c r="X1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>191</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" t="s">
+        <v>186</v>
+      </c>
+      <c r="S2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="1" customFormat="1">
+      <c r="A4" s="1">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="1" customFormat="1">
+      <c r="A5" s="1">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="1">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="1">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="S7" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="1"/>
+    <col min="9" max="9" width="20.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -2573,51 +3392,51 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Main Website,Incredible Connection"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"SAID,Passport"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -3035,16 +3854,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K7" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I7 O2:S7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I7 O2:S7" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M7" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L7" xr:uid="{00000000-0002-0000-0300-000003000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3053,20 +3872,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="9.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3195,25 +4014,141 @@
         <v>90</v>
       </c>
     </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>225503</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>225503</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>225503</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>225503</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>225503</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>225503</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F3E34B-74E1-42CB-89A3-AE1ED526C979}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3252,21 +4187,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3323,203 +4258,6 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1">
-      <c r="A2" s="1">
-        <v>99</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="1" customFormat="1">
-      <c r="A3" s="1">
-        <v>100</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3528,6 +4266,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3676,39 +4432,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3731,9 +4458,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TA93 cash demosit payment method added
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -1,36 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A508A08-E625-4376-88CD-627C33389085}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="15285" windowHeight="7875" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
     <sheet name="IC" sheetId="23" r:id="rId2"/>
-    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId3"/>
-    <sheet name="accountCreation++" sheetId="39" r:id="rId4"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId5"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId6"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId7"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId8"/>
-    <sheet name="Russels" sheetId="26" r:id="rId9"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId10"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId11"/>
-    <sheet name="Login++" sheetId="25" r:id="rId12"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId13"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId14"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId15"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId16"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId17"/>
+    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId3"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId4"/>
+    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId5"/>
+    <sheet name="accountCreation++" sheetId="39" r:id="rId6"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId7"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId8"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId9"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId10"/>
+    <sheet name="Russels" sheetId="26" r:id="rId11"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId12"/>
+    <sheet name="Login++" sheetId="25" r:id="rId13"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId14"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId15"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId16"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId17"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId18"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="174">
   <si>
     <t>testSuitID</t>
   </si>
@@ -302,9 +304,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Access#11</t>
-  </si>
-  <si>
     <t>general</t>
   </si>
   <si>
@@ -425,9 +424,6 @@
     <t>GenerateOrderSAPnumber</t>
   </si>
   <si>
-    <t>interval</t>
-  </si>
-  <si>
     <t>OrderID</t>
   </si>
   <si>
@@ -531,13 +527,40 @@
   </si>
   <si>
     <t>BPnumber</t>
+  </si>
+  <si>
+    <t>Magento Sales Using All Available Payment Methods</t>
+  </si>
+  <si>
+    <t>Cash_Deposits</t>
+  </si>
+  <si>
+    <t>ic_CashDepositPayment</t>
+  </si>
+  <si>
+    <t>Test Case name</t>
+  </si>
+  <si>
+    <t>Retrived OrderID</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>9108238533089</t>
+  </si>
+  <si>
+    <t>Access#1</t>
+  </si>
+  <si>
+    <t>TimeOutinSecond</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,8 +616,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -604,6 +633,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -636,7 +671,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -663,6 +698,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -725,6 +761,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -772,7 +811,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -805,9 +844,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -840,6 +896,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1015,21 +1088,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="4" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +1125,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1073,7 +1146,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1093,7 +1166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1113,7 +1186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1133,7 +1206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1153,7 +1226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1180,14 +1253,229 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD22"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" customWidth="1"/>
+    <col min="5" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1">
+      <c r="A2" s="1">
+        <v>99</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>100</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
@@ -1202,7 +1490,7 @@
     <col min="13" max="13" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>34</v>
       </c>
@@ -1243,9 +1531,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="5" customFormat="1">
       <c r="A2" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -1284,9 +1572,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="5" customFormat="1">
       <c r="A3" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -1322,12 +1610,12 @@
         <v>80</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="5" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -1363,92 +1651,71 @@
         <v>80</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="5" customFormat="1">
+      <c r="A5" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" s="5">
+        <v>2000</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="L4" r:id="rId3"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="L5" r:id="rId4" xr:uid="{3F0B0765-ADDA-4FFC-B11F-98D0481214B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
@@ -1456,7 +1723,7 @@
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1470,7 +1737,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1484,7 +1751,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1498,7 +1765,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="1" customFormat="1">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1512,7 +1779,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="1" customFormat="1">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1526,7 +1793,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="1" customFormat="1">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1540,7 +1807,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="1" customFormat="1">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -1554,7 +1821,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="1" customFormat="1">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -1568,7 +1835,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="1" customFormat="1">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -1582,7 +1849,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="1" customFormat="1">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -1596,7 +1863,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="1" customFormat="1">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -1610,7 +1877,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="1" customFormat="1">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -1624,7 +1891,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="1" customFormat="1">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -1644,15 +1911,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -1664,7 +1931,7 @@
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
@@ -1690,12 +1957,12 @@
         <v>54</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1">
       <c r="A2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1719,9 +1986,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="4" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -1745,9 +2012,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="4" customFormat="1">
       <c r="A4" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -1777,15 +2044,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
@@ -1795,7 +2062,7 @@
     <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1836,7 +2103,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1856,7 +2123,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1881,15 +2148,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
@@ -1899,7 +2166,7 @@
     <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1940,7 +2207,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1960,7 +2227,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1985,15 +2252,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
@@ -2003,7 +2270,7 @@
     <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2044,7 +2311,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2064,7 +2331,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2089,15 +2356,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="L14" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
@@ -2107,7 +2374,7 @@
     <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2148,7 +2415,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2168,7 +2435,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2194,14 +2461,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView topLeftCell="F2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="55.28515625" style="10" bestFit="1" customWidth="1"/>
@@ -2210,8 +2477,8 @@
     <col min="7" max="7" width="28.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
@@ -2219,12 +2486,12 @@
     <col min="16" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>16</v>
@@ -2233,7 +2500,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>17</v>
@@ -2266,15 +2533,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="10">
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -2295,171 +2562,206 @@
         <v>33</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" s="1" customFormat="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="1" customFormat="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>8</v>
+        <v>141</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="1" customFormat="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="1" customFormat="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="1" customFormat="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="17">
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G9" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="17">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>165</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2484,14 +2786,134 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD085654-08FC-4AEB-8740-0EA07D698CB8}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="1" customFormat="1">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
@@ -2507,7 +2929,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -2515,34 +2937,34 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>8</v>
       </c>
@@ -2550,22 +2972,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E2" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="J2" s="1">
         <v>11</v>
@@ -2573,30 +2995,30 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Main Website,Incredible Connection"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"SAID,Passport"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -2620,7 +3042,7 @@
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -2628,58 +3050,58 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>71</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -2687,58 +3109,58 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J2" s="1">
         <v>2222224</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>111</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -2746,58 +3168,58 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J3" s="1">
         <v>2222224</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N3" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>111</v>
-      </c>
       <c r="O3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -2805,58 +3227,58 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J4" s="1">
         <v>2222225</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N4" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>111</v>
-      </c>
       <c r="O4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -2864,58 +3286,58 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J5" s="1">
         <v>2222226</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N5" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>111</v>
-      </c>
       <c r="O5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -2923,58 +3345,58 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J6" s="1">
         <v>2222227</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="P6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -2982,69 +3404,69 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J7" s="1">
         <v>2222228</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N7" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>111</v>
-      </c>
       <c r="O7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K7" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I7 O2:S7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I7 O2:S7" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M7" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L7" xr:uid="{00000000-0002-0000-0300-000003000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3053,15 +3475,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D2" sqref="D2:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
@@ -3069,7 +3491,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -3083,7 +3505,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3094,10 +3516,10 @@
         <v>225564</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3108,10 +3530,10 @@
         <v>225564</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3122,10 +3544,10 @@
         <v>225564</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3136,10 +3558,10 @@
         <v>225564</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3150,10 +3572,10 @@
         <v>225564</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3164,10 +3586,10 @@
         <v>225564</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3178,10 +3600,10 @@
         <v>225564</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3192,7 +3614,89 @@
         <v>225564</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>90</v>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>225564</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -3200,67 +3704,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
@@ -3269,7 +3721,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -3277,13 +3729,13 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3294,10 +3746,10 @@
         <v>3100000680</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3308,10 +3760,10 @@
         <v>3100000680</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3322,204 +3774,7 @@
         <v>3100000680</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>99</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>100</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3528,6 +3783,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3676,25 +3949,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3711,29 +3991,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Redeem the gift card as the guest user or registered user
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -3,36 +3,40 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A508A08-E625-4376-88CD-627C33389085}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60977545-4D91-4CF5-AEB7-D64DD153FFC1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1770" windowWidth="15285" windowHeight="7875" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="16780" windowHeight="9880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
     <sheet name="IC" sheetId="23" r:id="rId2"/>
-    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId3"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId4"/>
-    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId5"/>
-    <sheet name="accountCreation++" sheetId="39" r:id="rId6"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId7"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId8"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId9"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId10"/>
-    <sheet name="Russels" sheetId="26" r:id="rId11"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId12"/>
-    <sheet name="Login++" sheetId="25" r:id="rId13"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId14"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId15"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId16"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId17"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId18"/>
+    <sheet name="ic_login++" sheetId="46" r:id="rId3"/>
+    <sheet name="icRedeemGiftCard++" sheetId="45" r:id="rId4"/>
+    <sheet name="adminUserUpdate++" sheetId="43" r:id="rId5"/>
+    <sheet name="icGiftCardPurchase++" sheetId="44" r:id="rId6"/>
+    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId7"/>
+    <sheet name="accountCreation++" sheetId="39" r:id="rId8"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId9"/>
+    <sheet name="customerValidationUpdates++" sheetId="42" r:id="rId10"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId11"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId12"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId13"/>
+    <sheet name="Russels" sheetId="26" r:id="rId14"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId15"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId16"/>
+    <sheet name="Login++" sheetId="25" r:id="rId17"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId18"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId19"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId20"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId21"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId22"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="243">
   <si>
     <t>testSuitID</t>
   </si>
@@ -151,12 +155,6 @@
     <t>typeSearch</t>
   </si>
   <si>
-    <t>categorySearch</t>
-  </si>
-  <si>
-    <t>productsToSearch</t>
-  </si>
-  <si>
     <t>specificProduct</t>
   </si>
   <si>
@@ -217,9 +215,6 @@
     <t>iCcartVerification</t>
   </si>
   <si>
-    <t>searchbar</t>
-  </si>
-  <si>
     <t>deliveryPopulation</t>
   </si>
   <si>
@@ -304,19 +299,7 @@
     <t>Password</t>
   </si>
   <si>
-    <t>general</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>Photography </t>
-  </si>
-  <si>
-    <t>CANON DIGITAL CAM IXUS 185 BLACK</t>
-  </si>
-  <si>
-    <t>OFA SAMSUNG REMOTE URC1910</t>
+    <t>Access#11</t>
   </si>
   <si>
     <t>Create Sales order with guest user- using product search bar</t>
@@ -352,12 +335,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>sumsung</t>
-  </si>
-  <si>
-    <t>Samsung Toner D105L</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -424,6 +401,9 @@
     <t>GenerateOrderSAPnumber</t>
   </si>
   <si>
+    <t>interval</t>
+  </si>
+  <si>
     <t>OrderID</t>
   </si>
   <si>
@@ -529,31 +509,262 @@
     <t>BPnumber</t>
   </si>
   <si>
-    <t>Magento Sales Using All Available Payment Methods</t>
-  </si>
-  <si>
-    <t>Cash_Deposits</t>
-  </si>
-  <si>
-    <t>ic_CashDepositPayment</t>
-  </si>
-  <si>
-    <t>Test Case name</t>
-  </si>
-  <si>
-    <t>Retrived OrderID</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>9108238533089</t>
-  </si>
-  <si>
-    <t>Access#1</t>
-  </si>
-  <si>
-    <t>TimeOutinSecond</t>
+    <t>adminFirstName_output</t>
+  </si>
+  <si>
+    <t>adminLastName_output</t>
+  </si>
+  <si>
+    <t>taxVat</t>
+  </si>
+  <si>
+    <t>adminTaxVat_output</t>
+  </si>
+  <si>
+    <t>adminEmail_output</t>
+  </si>
+  <si>
+    <t>billingAddress</t>
+  </si>
+  <si>
+    <t>billing_streetAddress</t>
+  </si>
+  <si>
+    <t>billing_buildingDetails_output</t>
+  </si>
+  <si>
+    <t>billing_provinceName_output</t>
+  </si>
+  <si>
+    <t>billing_city_output</t>
+  </si>
+  <si>
+    <t>billing_suburb_output</t>
+  </si>
+  <si>
+    <t>billing_postalCode_output</t>
+  </si>
+  <si>
+    <t>shippingAddress</t>
+  </si>
+  <si>
+    <t>shipping_buildingDetails_output</t>
+  </si>
+  <si>
+    <t>shipping_provinceName_output</t>
+  </si>
+  <si>
+    <t>shipping_city_output</t>
+  </si>
+  <si>
+    <t>shipping_suburb_output</t>
+  </si>
+  <si>
+    <t>shipping_postalCode_output</t>
+  </si>
+  <si>
+    <t>Northern Cape</t>
+  </si>
+  <si>
+    <t>adminUserUpdate</t>
+  </si>
+  <si>
+    <t>Update customer information on Magento</t>
+  </si>
+  <si>
+    <t>Bongi</t>
+  </si>
+  <si>
+    <t>shipping_streetAddress</t>
+  </si>
+  <si>
+    <t>LauraPLittle@teleworm.us</t>
+  </si>
+  <si>
+    <t>adminShipping_streetAddress_Output</t>
+  </si>
+  <si>
+    <t>Update customer information Mangento All update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updating customer first name on Magento </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updating customer last name on Magento  </t>
+  </si>
+  <si>
+    <t>Updating customer's email on Magento</t>
+  </si>
+  <si>
+    <t>Updating customer's billing address on Magento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updating customers shipping on Magento </t>
+  </si>
+  <si>
+    <t>selectAmount</t>
+  </si>
+  <si>
+    <t>inputAmount</t>
+  </si>
+  <si>
+    <t>senderName</t>
+  </si>
+  <si>
+    <t>senderEmail</t>
+  </si>
+  <si>
+    <t>recipientName</t>
+  </si>
+  <si>
+    <t>recipientEmail</t>
+  </si>
+  <si>
+    <t>cardMessage</t>
+  </si>
+  <si>
+    <t>R100</t>
+  </si>
+  <si>
+    <t>selectAmountFlag</t>
+  </si>
+  <si>
+    <t>Gift card purchase</t>
+  </si>
+  <si>
+    <t>icGiftCardPurchase</t>
+  </si>
+  <si>
+    <t>ic_login</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>cartButtonWaitTimeInSeconds</t>
+  </si>
+  <si>
+    <t>SearchUsingSearchBar</t>
+  </si>
+  <si>
+    <t>All Products</t>
+  </si>
+  <si>
+    <t>JBL EARPHONE T110 BLUE#Xbox One Stealth 600 Gaming Headsets#APPLE TV 4K 64GB MP7P2SOA#OFA 8 In 1 Universal Remote URC1280</t>
+  </si>
+  <si>
+    <t>2#1#2#4</t>
+  </si>
+  <si>
+    <t>Cellphones &amp; Accessories</t>
+  </si>
+  <si>
+    <t>Snug Car Juice 3.4A Charger Light Cable - Black#Snug 8000mAh Powerbank LCD Quick Charge Black#SNUG MFI LIGHTING CABLE 1.2M-WHITE</t>
+  </si>
+  <si>
+    <t>2#3#1</t>
+  </si>
+  <si>
+    <t>Computers Notebooks &amp; Tablet's</t>
+  </si>
+  <si>
+    <t>SNUG MFI LIGHTING CABLE 2M-WHITE#Solo Urban Metro Universal Fit 5.5-8.5-inch Tablet Case - Bl#Body Glove Apple iPad 9.7-inch (2017) Smartsuit-Black</t>
+  </si>
+  <si>
+    <t>3#1#2</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B40</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B41</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B42</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B43</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B44</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B45</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B46</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B47</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B48</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B49</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B50</t>
+  </si>
+  <si>
+    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B51</t>
+  </si>
+  <si>
+    <t>icRedeemGiftCard</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>giftCardCode</t>
+  </si>
+  <si>
+    <t>scratchCode</t>
+  </si>
+  <si>
+    <t>Redeem the gift card by guest user</t>
+  </si>
+  <si>
+    <t>Redeem the gift card by Registered user</t>
+  </si>
+  <si>
+    <t>JBL Endurance Sprint - Black</t>
+  </si>
+  <si>
+    <t>BonginhlanhlaM@jdg.co.za</t>
+  </si>
+  <si>
+    <t>Password@123</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Hugo Boss</t>
+  </si>
+  <si>
+    <t>Red Door</t>
+  </si>
+  <si>
+    <t>We like smelliong good</t>
+  </si>
+  <si>
+    <t>X8QDX4WTKL4ZT6P</t>
+  </si>
+  <si>
+    <t>E93FJ</t>
+  </si>
+  <si>
+    <t>9012022605089</t>
+  </si>
+  <si>
+    <t>FD3A3TX4QXAL3QN</t>
+  </si>
+  <si>
+    <t>TWV4N</t>
+  </si>
+  <si>
+    <t>icExistingAddress</t>
   </si>
 </sst>
 </file>
@@ -623,7 +834,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -633,12 +844,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -671,7 +876,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -698,7 +903,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1095,11 +1299,11 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" customWidth="1"/>
+    <col min="4" max="6" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1253,20 +1457,181 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F3E34B-74E1-42CB-89A3-AE1ED526C979}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3100000680</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3100000680</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3100000680</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="130.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1283,78 +1648,209 @@
         <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>107</v>
+        <v>202</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>94</v>
+        <v>202</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>91</v>
+        <v>203</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1">
       <c r="C5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>206</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>107</v>
-      </c>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1362,7 +1858,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -1370,15 +1866,15 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
@@ -1386,7 +1882,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>16</v>
@@ -1467,7 +1963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
@@ -1475,19 +1971,19 @@
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="5" customFormat="1">
@@ -1498,201 +1994,201 @@
         <v>35</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1">
       <c r="A2" s="5" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="J2" s="5">
         <v>2000</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1">
       <c r="A3" s="5" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="J3" s="5">
         <v>2000</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="J4" s="5">
         <v>2000</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>99</v>
+        <v>225</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="J5" s="5">
         <v>2000</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>171</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -1700,14 +2196,99 @@
     <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
     <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
     <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
-    <hyperlink ref="L5" r:id="rId4" xr:uid="{3F0B0765-ADDA-4FFC-B11F-98D0481214B0}"/>
+    <hyperlink ref="L5" r:id="rId4" xr:uid="{819E883A-3011-4D0C-9045-354176492D46}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="11.26953125" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="1" customFormat="1">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="1" customFormat="1">
+      <c r="A5" s="3">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="1" customFormat="1">
+      <c r="A6" s="3">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -1715,12 +2296,12 @@
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
@@ -1731,10 +2312,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1745,10 +2326,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1759,10 +2340,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1">
@@ -1773,10 +2354,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1">
@@ -1787,10 +2368,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1">
@@ -1801,10 +2382,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1">
@@ -1815,10 +2396,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1">
@@ -1829,10 +2410,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1">
@@ -1843,10 +2424,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1">
@@ -1857,10 +2438,10 @@
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1">
@@ -1871,10 +2452,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1">
@@ -1885,10 +2466,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1">
@@ -1899,10 +2480,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1911,24 +2492,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
     <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
@@ -1939,103 +2520,155 @@
         <v>35</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1">
       <c r="A2" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="4" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1">
       <c r="A4" s="4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="4" customFormat="1">
+      <c r="A5" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>55</v>
+      <c r="F5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="4" customFormat="1">
+      <c r="A6" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2044,7 +2677,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -2052,14 +2685,14 @@
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -2108,19 +2741,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1">
@@ -2128,331 +2761,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView topLeftCell="L14" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2462,28 +2783,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView topLeftCell="F2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="55.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="10.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="55.26953125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="25.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.90625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.26953125" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.1796875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2491,7 +2812,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>16</v>
@@ -2500,7 +2821,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>17</v>
@@ -2538,10 +2859,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -2550,10 +2871,10 @@
         <v>31</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>32</v>
@@ -2562,13 +2883,13 @@
         <v>33</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1">
@@ -2576,19 +2897,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1">
@@ -2596,22 +2917,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="1" customFormat="1">
@@ -2619,22 +2940,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="1" customFormat="1">
@@ -2642,22 +2963,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="16" t="s">
         <v>140</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="1" customFormat="1">
@@ -2665,22 +2986,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="1" customFormat="1">
@@ -2688,22 +3009,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -2711,22 +3032,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D9" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -2734,34 +3055,234 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="D10" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="17">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="17">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="17">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="17">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="17">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="17">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="17">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="F10" s="18" t="s">
+      <c r="E18" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="9" t="s">
+      <c r="H18" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="J18" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>129</v>
+      <c r="K18" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2785,45 +3306,372 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD085654-08FC-4AEB-8740-0EA07D698CB8}">
-  <dimension ref="A1:D2"/>
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView topLeftCell="L14" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F804F0DF-BCF2-495B-87D7-DE13736AAC9A}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="3" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>169</v>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="3">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>165</v>
+      <c r="A2">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2832,72 +3680,398 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC768DC-A877-40A8-842F-EF3C3A088513}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="1" customFormat="1">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C59FE87-E0B0-46B2-B1F3-245D04193D71}">
+  <dimension ref="A1:Y7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M1" t="s">
+        <v>164</v>
+      </c>
+      <c r="N1" t="s">
+        <v>165</v>
+      </c>
+      <c r="O1" t="s">
         <v>166</v>
+      </c>
+      <c r="P1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R1" t="s">
+        <v>169</v>
+      </c>
+      <c r="S1" t="s">
+        <v>179</v>
+      </c>
+      <c r="T1" t="s">
+        <v>181</v>
+      </c>
+      <c r="U1" t="s">
+        <v>170</v>
+      </c>
+      <c r="V1" t="s">
+        <v>171</v>
+      </c>
+      <c r="W1" t="s">
+        <v>172</v>
+      </c>
+      <c r="X1" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" t="s">
+        <v>175</v>
+      </c>
+      <c r="R2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" s="1" customFormat="1">
+      <c r="A4" s="1">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="1" customFormat="1">
+      <c r="A5" s="1">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" s="1">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" s="1">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="R7" t="s">
+        <v>8</v>
+      </c>
+      <c r="S7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2905,7 +4079,104 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC6242C-70B0-4EE9-8BAD-E933762B0B6F}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="3" width="15.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I1" t="s">
+        <v>193</v>
+      </c>
+      <c r="J1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E2">
+        <v>500</v>
+      </c>
+      <c r="F2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H2" t="s">
+        <v>235</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="J2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{E2639DC8-C7C7-408C-B7BB-8F6985325174}">
+      <formula1>"R100,R200,R300,R400,R500"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{F8A295CC-30BF-49BD-9777-7A8EE14F2666}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -2913,20 +4184,20 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="1"/>
+    <col min="9" max="9" width="20.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -2937,31 +4208,31 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -2972,22 +4243,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="J2" s="1">
         <v>11</v>
@@ -3010,36 +4281,36 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -3050,55 +4321,55 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -3109,55 +4380,55 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="J2" s="1">
         <v>2222224</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -3168,55 +4439,55 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="J3" s="1">
         <v>2222224</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -3227,55 +4498,55 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="J4" s="1">
         <v>2222225</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -3286,55 +4557,55 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="J5" s="1">
         <v>2222226</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -3345,55 +4616,55 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>147</v>
-      </c>
       <c r="G6" s="14" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="J6" s="1">
         <v>2222227</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -3404,55 +4675,55 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="J7" s="1">
         <v>2222228</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -3475,20 +4746,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="9.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3499,10 +4770,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3516,7 +4787,7 @@
         <v>225564</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>172</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3530,7 +4801,7 @@
         <v>225564</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>172</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3544,7 +4815,7 @@
         <v>225564</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>172</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3558,7 +4829,7 @@
         <v>225564</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>172</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3572,7 +4843,7 @@
         <v>225564</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>172</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -3586,7 +4857,7 @@
         <v>225564</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>172</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3600,7 +4871,7 @@
         <v>225564</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>172</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -3614,7 +4885,7 @@
         <v>225564</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>172</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3625,10 +4896,80 @@
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>225564</v>
+        <v>225503</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>172</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>225503</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>225503</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>225503</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>225503</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>225503</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3637,170 +4978,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1">
-        <v>240</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>3100000680</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>3100000680</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3100000680</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3949,32 +5127,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3991,4 +5162,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update inputsheet gift card
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -4,34 +4,36 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1770" windowWidth="15285" windowHeight="7875" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="15285" windowHeight="7875" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
     <sheet name="IC" sheetId="23" r:id="rId2"/>
-    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId3"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId4"/>
-    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId5"/>
-    <sheet name="accountCreation++" sheetId="39" r:id="rId6"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId7"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId8"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId9"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId10"/>
-    <sheet name="Russels" sheetId="26" r:id="rId11"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId12"/>
-    <sheet name="Login++" sheetId="25" r:id="rId13"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId14"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId15"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId16"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId17"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId18"/>
+    <sheet name="ic_login++" sheetId="44" r:id="rId3"/>
+    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId4"/>
+    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId5"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId6"/>
+    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId7"/>
+    <sheet name="accountCreation++" sheetId="39" r:id="rId8"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId9"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId10"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId11"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId12"/>
+    <sheet name="Russels" sheetId="26" r:id="rId13"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId14"/>
+    <sheet name="Login++" sheetId="25" r:id="rId15"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId16"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId17"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId18"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId19"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId20"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="222">
   <si>
     <t>testSuitID</t>
   </si>
@@ -598,6 +600,105 @@
   </si>
   <si>
     <t>Password4</t>
+  </si>
+  <si>
+    <t>Gift card purchase</t>
+  </si>
+  <si>
+    <t>ic_login</t>
+  </si>
+  <si>
+    <t>icGiftCardPurchase</t>
+  </si>
+  <si>
+    <t>selectAmountFlag</t>
+  </si>
+  <si>
+    <t>selectAmount</t>
+  </si>
+  <si>
+    <t>inputAmount</t>
+  </si>
+  <si>
+    <t>senderName</t>
+  </si>
+  <si>
+    <t>senderEmail</t>
+  </si>
+  <si>
+    <t>recipientName</t>
+  </si>
+  <si>
+    <t>recipientEmail</t>
+  </si>
+  <si>
+    <t>cardMessage</t>
+  </si>
+  <si>
+    <t>R200</t>
+  </si>
+  <si>
+    <t>Rashad</t>
+  </si>
+  <si>
+    <t>Bonginhlanhla.Mazibuko@itcinfotech.com</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>BonginhlanhlaM@jdg.co.za</t>
+  </si>
+  <si>
+    <t>Happy birthday big boss</t>
+  </si>
+  <si>
+    <t>R100</t>
+  </si>
+  <si>
+    <t>Hugo Boss</t>
+  </si>
+  <si>
+    <t>Red Door</t>
+  </si>
+  <si>
+    <t>We like smelling good</t>
+  </si>
+  <si>
+    <t>Nike Just</t>
+  </si>
+  <si>
+    <t>Addidas Sporty</t>
+  </si>
+  <si>
+    <t>we are sport wear.</t>
+  </si>
+  <si>
+    <t>Samsung fone</t>
+  </si>
+  <si>
+    <t>Iphone Apple</t>
+  </si>
+  <si>
+    <t>we are phone leading brands</t>
+  </si>
+  <si>
+    <t>JBL headset</t>
+  </si>
+  <si>
+    <t>Sony headset</t>
+  </si>
+  <si>
+    <t>we are headsets</t>
+  </si>
+  <si>
+    <t>Password@123</t>
+  </si>
+  <si>
+    <t>LauraPLittle@teleworm.us</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -715,7 +816,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -743,6 +844,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1264,6 +1367,179 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1">
+      <c r="A4" s="1">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3100000680</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3100000680</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3100000680</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3100000680</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1532,7 +1808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -1637,7 +1913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
@@ -1877,7 +2153,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -2081,12 +2357,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2208,13 +2484,39 @@
         <v>53</v>
       </c>
     </row>
+    <row r="5" spans="1:9" s="4" customFormat="1">
+      <c r="A5" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -2318,7 +2620,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -2422,7 +2724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -2526,133 +2828,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView topLeftCell="L14" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="C2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O10"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="55.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="59.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="27.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
@@ -2933,6 +3130,45 @@
       <c r="K10" s="10" t="s">
         <v>119</v>
       </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="9">
+        <v>15</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
@@ -2955,7 +3191,405 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView topLeftCell="L14" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="9">
+        <v>15</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" s="9">
+        <v>300</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="9">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" s="9">
+        <v>500</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="9">
+        <v>15</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E4" s="9">
+        <v>100</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="9">
+        <v>15</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E5" s="9">
+        <v>400</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="9">
+        <v>15</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E6" s="9">
+        <v>350</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3001,12 +3635,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3070,12 +3704,23 @@
         <v>156</v>
       </c>
     </row>
+    <row r="6" spans="1:3" s="1" customFormat="1">
+      <c r="A6" s="1">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -3180,7 +3825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S7"/>
   <sheetViews>
@@ -3645,12 +4290,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3801,153 +4446,22 @@
         <v>188</v>
       </c>
     </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>225505</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1">
-        <v>240</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>3100000680</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>3100000680</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3100000680</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Login to IC login
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1770" windowWidth="15285" windowHeight="7875" activeTab="3"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="15285" windowHeight="7875" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="220">
   <si>
     <t>testSuitID</t>
   </si>
@@ -658,9 +658,6 @@
   </si>
   <si>
     <t>AutoJDGTest@gmail.com</t>
-  </si>
-  <si>
-    <t>AutoJDGTest2@gmail.com</t>
   </si>
   <si>
     <t>Gift card purchase verifiacation Sender</t>
@@ -2902,8 +2899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2914,7 +2911,7 @@
     <col min="5" max="5" width="12.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="28.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="27.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
@@ -3244,23 +3241,29 @@
         <v>16</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+        <v>190</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
@@ -3562,8 +3565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3589,31 +3592,31 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -3627,7 +3630,7 @@
         <v>207</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H2" s="1">
         <v>300</v>
@@ -3643,8 +3646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3714,7 +3717,7 @@
         <v>201</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>202</v>
@@ -4437,21 +4440,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4604,6 +4607,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -4616,14 +4627,6 @@
     <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
main update inpursheet update
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -4,37 +4,41 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1770" windowWidth="15285" windowHeight="7875" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="15285" windowHeight="7875" firstSheet="13" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
     <sheet name="IC" sheetId="23" r:id="rId2"/>
-    <sheet name="ic_login++" sheetId="44" r:id="rId3"/>
-    <sheet name="icGiftCardVerificationSender++" sheetId="45" r:id="rId4"/>
-    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId5"/>
-    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId6"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId7"/>
-    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId8"/>
-    <sheet name="accountCreation++" sheetId="39" r:id="rId9"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId10"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId11"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId12"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId13"/>
-    <sheet name="Russels" sheetId="26" r:id="rId14"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId15"/>
-    <sheet name="Login++" sheetId="25" r:id="rId16"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId17"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId18"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId19"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId20"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId21"/>
+    <sheet name="icRedeemGiftCard++" sheetId="48" r:id="rId3"/>
+    <sheet name="VeriyGiftcardUsableity++" sheetId="49" r:id="rId4"/>
+    <sheet name="ic_login++" sheetId="44" r:id="rId5"/>
+    <sheet name="SAP_OrderRelated++" sheetId="46" r:id="rId6"/>
+    <sheet name="DB_connection_master++" sheetId="47" r:id="rId7"/>
+    <sheet name="icGiftCardVerificationSender++" sheetId="45" r:id="rId8"/>
+    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId9"/>
+    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId10"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId11"/>
+    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId12"/>
+    <sheet name="accountCreation++" sheetId="39" r:id="rId13"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId14"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId15"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId16"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId17"/>
+    <sheet name="Russels" sheetId="26" r:id="rId18"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId19"/>
+    <sheet name="Login++" sheetId="25" r:id="rId20"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId21"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId22"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId23"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId24"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId25"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="251">
   <si>
     <t>testSuitID</t>
   </si>
@@ -597,9 +601,6 @@
     <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B50</t>
   </si>
   <si>
-    <t>Sandisk Cruzer Blade USB 16GB SDCZ50-016G-B51</t>
-  </si>
-  <si>
     <t>Password4</t>
   </si>
   <si>
@@ -660,12 +661,6 @@
     <t>AutoJDGTest@gmail.com</t>
   </si>
   <si>
-    <t>Gift card purchase verifiacation Sender</t>
-  </si>
-  <si>
-    <t>icGiftCardVerificationSender</t>
-  </si>
-  <si>
     <t>reciever</t>
   </si>
   <si>
@@ -693,17 +688,116 @@
     <t>emailCountAfterGiftCardBuy</t>
   </si>
   <si>
-    <t>getnumberOfEmails</t>
-  </si>
-  <si>
     <t>16</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>port</t>
+  </si>
+  <si>
+    <t>TypeOfDB</t>
+  </si>
+  <si>
+    <t>DB_Instance</t>
+  </si>
+  <si>
+    <t>ECCQA</t>
+  </si>
+  <si>
+    <t>HANA</t>
+  </si>
+  <si>
+    <t>11.19.2.172</t>
+  </si>
+  <si>
+    <t>Welc0me@2021</t>
+  </si>
+  <si>
+    <t>ECCPROD</t>
+  </si>
+  <si>
+    <t>CRMQA</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>11.19.0.68</t>
+  </si>
+  <si>
+    <t>1433 </t>
+  </si>
+  <si>
+    <t>cq1adm</t>
+  </si>
+  <si>
+    <t>#D3*t3R#</t>
+  </si>
+  <si>
+    <t>CRMPROD</t>
+  </si>
+  <si>
+    <t>Create Customer Account from Sales Order</t>
+  </si>
+  <si>
+    <t>SAP_OrderRelated</t>
+  </si>
+  <si>
+    <t>Bongi</t>
+  </si>
+  <si>
+    <t>icRedeemGiftCard</t>
+  </si>
+  <si>
+    <t>Redeem the gift card by Registered user</t>
+  </si>
+  <si>
+    <t>icExistingAddress</t>
+  </si>
+  <si>
+    <t>giftCardCode</t>
+  </si>
+  <si>
+    <t>X8QDX4WTKL4ZT6P</t>
+  </si>
+  <si>
+    <t>E93FJ</t>
+  </si>
+  <si>
+    <t>FD3A3TX4QXAL3QN</t>
+  </si>
+  <si>
+    <t>TWV4N</t>
+  </si>
+  <si>
+    <t>DelayTime</t>
+  </si>
+  <si>
+    <t>GiftcardCode</t>
+  </si>
+  <si>
+    <t>ScratchCode</t>
+  </si>
+  <si>
+    <t>ExpBalance</t>
+  </si>
+  <si>
+    <t>VeriyGiftcardUsableity</t>
+  </si>
+  <si>
+    <t>Veriy Gift card Usableity</t>
+  </si>
+  <si>
+    <t>Samsung Toner D105L</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -765,6 +859,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF212121"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -814,7 +914,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -844,6 +944,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1206,14 +1307,14 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="4" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1236,7 +1337,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1257,7 +1358,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1277,7 +1378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1297,7 +1398,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1317,7 +1418,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1337,7 +1438,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1365,13 +1466,725 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="1" customFormat="1">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="1" customFormat="1">
+      <c r="A6" s="1">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" s="1">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
+      <formula1>"Main Website,Incredible Connection"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
+      <formula1>"SAID,Passport"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="TestAutomation2@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S7"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="1">
+        <v>2222224</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2222224</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2222225</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" s="1">
+        <v>2222226</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2222227</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2222228</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K7">
+      <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I7 O2:S7">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M7">
+      <formula1>"ID, Passport"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L7">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
@@ -1379,7 +2192,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1393,7 +2206,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1404,10 +2217,10 @@
         <v>225505</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1418,10 +2231,10 @@
         <v>225505</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1432,10 +2245,10 @@
         <v>225505</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1446,10 +2259,10 @@
         <v>225505</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1460,10 +2273,10 @@
         <v>225505</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1474,10 +2287,10 @@
         <v>225505</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1488,10 +2301,10 @@
         <v>225505</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1502,10 +2315,10 @@
         <v>225505</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1516,10 +2329,10 @@
         <v>225505</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>15</v>
       </c>
@@ -1530,7 +2343,7 @@
         <v>225505</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1539,15 +2352,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
@@ -1556,7 +2369,7 @@
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1573,7 +2386,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1587,7 +2400,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>9</v>
       </c>
@@ -1601,7 +2414,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="1" customFormat="1">
       <c r="A4" s="1">
         <v>15</v>
       </c>
@@ -1620,15 +2433,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
@@ -1637,7 +2450,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1651,7 +2464,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1665,7 +2478,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1679,7 +2492,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1693,7 +2506,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>15</v>
       </c>
@@ -1712,15 +2525,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
@@ -1730,7 +2543,7 @@
     <col min="6" max="6" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1750,7 +2563,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="1" customFormat="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1770,7 +2583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1790,7 +2603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="1" customFormat="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1806,8 +2619,11 @@
       <c r="E4" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -1823,8 +2639,11 @@
       <c r="E5" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -1840,8 +2659,11 @@
       <c r="E6" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -1854,126 +2676,231 @@
       <c r="D7" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>11</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>12</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>13</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="1">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="1">
+        <v>2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>16</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
+      <c r="C16" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>17</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <v>2</v>
+      </c>
+      <c r="F17" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>18</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>187</v>
+      <c r="C18" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1982,7 +2909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -1990,7 +2917,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
@@ -2001,7 +2928,7 @@
     <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2045,7 +2972,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="1" customFormat="1">
       <c r="A2" s="1">
         <v>99</v>
       </c>
@@ -2065,7 +2992,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>100</v>
       </c>
@@ -2087,15 +3014,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
@@ -2110,7 +3037,7 @@
     <col min="13" max="13" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>34</v>
       </c>
@@ -2151,7 +3078,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="5" customFormat="1">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -2192,7 +3119,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="5" customFormat="1">
       <c r="A3" s="5" t="s">
         <v>96</v>
       </c>
@@ -2233,7 +3160,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="5" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>97</v>
       </c>
@@ -2274,7 +3201,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="5" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>160</v>
       </c>
@@ -2315,9 +3242,9 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="5" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>91</v>
@@ -2350,7 +3277,7 @@
         <v>76</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>161</v>
@@ -2369,612 +3296,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:I12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="59.5703125" style="10" bestFit="1" customWidth="1"/>
@@ -2982,15 +3312,13 @@
     <col min="5" max="5" width="12.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="28.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="27.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="28.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="27.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
@@ -3037,7 +3365,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -3074,8 +3402,11 @@
       <c r="M2" s="10" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N2" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3095,7 +3426,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="1" customFormat="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3118,7 +3449,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="1" customFormat="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3141,7 +3472,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="1" customFormat="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3164,7 +3495,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="1" customFormat="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3187,7 +3518,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="1" customFormat="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3210,7 +3541,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="17">
         <v>8</v>
       </c>
@@ -3233,7 +3564,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="17">
         <v>9</v>
       </c>
@@ -3268,25 +3599,25 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="9">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>190</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>191</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>32</v>
@@ -3307,40 +3638,69 @@
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>16</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="D12" s="9" t="s">
+    <row r="12" spans="1:15">
+      <c r="A12" s="17">
+        <v>17</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="17">
+        <v>18</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
+      <c r="F13" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>248</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
@@ -3365,13 +3725,402 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="4" customFormat="1">
+      <c r="A3" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="4" customFormat="1">
+      <c r="A4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="4" customFormat="1">
+      <c r="A5" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="4" customFormat="1">
+      <c r="A6" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
@@ -3381,7 +4130,7 @@
     <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3422,7 +4171,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3442,7 +4191,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3467,15 +4216,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView topLeftCell="L14" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
@@ -3485,7 +4234,7 @@
     <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3526,7 +4275,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3546,7 +4295,215 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView topLeftCell="L14" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3576,10 +4533,157 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>100</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="48.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -3587,7 +4691,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -3601,7 +4705,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>15</v>
       </c>
@@ -3609,13 +4713,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>16</v>
       </c>
@@ -3623,9 +4727,37 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D3" s="20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>126</v>
       </c>
     </row>
@@ -3638,15 +4770,188 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2" s="16">
+        <v>30215</v>
+      </c>
+      <c r="E2" s="16">
+        <v>225505</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="G4" s="16"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
@@ -3661,7 +4966,7 @@
     <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -3669,48 +4974,65 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1">
+      <c r="A2" s="1">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="H2" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1">
         <v>16</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H2" s="1">
-        <v>300</v>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H3" s="1">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -3719,7 +5041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -3727,7 +5049,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="10" bestFit="1" customWidth="1"/>
@@ -3742,7 +5064,7 @@
     <col min="11" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="9" t="s">
         <v>34</v>
       </c>
@@ -3750,31 +5072,31 @@
         <v>35</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="9">
         <v>15</v>
       </c>
@@ -3785,28 +5107,28 @@
         <v>99</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E2" s="9">
         <v>300</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="G2" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="I2" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="9">
         <v>16</v>
       </c>
@@ -3817,25 +5139,25 @@
         <v>99</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E3" s="9">
         <v>300</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="G3" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>202</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3849,728 +5171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="J2" s="1">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
-      <formula1>"Main Website,Incredible Connection"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
-      <formula1>"SAID,Passport"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="TestAutomation2@gmail.com"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S7"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J2" s="1">
-        <v>2222224</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J3" s="1">
-        <v>2222224</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J4" s="1">
-        <v>2222225</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J5" s="1">
-        <v>2222226</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J6" s="1">
-        <v>2222227</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J7" s="1">
-        <v>2222228</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K7">
-      <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I7 O2:S7">
-      <formula1>"Yes, No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M7">
-      <formula1>"ID, Passport"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L7">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4579,7 +5180,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4728,24 +5329,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4753,7 +5346,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4770,4 +5363,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated customer magento creation back end, customer update magento back
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE93B7E-F8BD-4C53-85FA-6B6C3566A8AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B799C7EB-4223-4E3D-93AA-EB624070366C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
@@ -14,31 +14,32 @@
     <sheet name="SapCustomer++" sheetId="45" r:id="rId4"/>
     <sheet name="SAP_OrderRelated++" sheetId="48" r:id="rId5"/>
     <sheet name="ICUpdateUser++" sheetId="49" r:id="rId6"/>
-    <sheet name="ic_login++" sheetId="44" r:id="rId7"/>
-    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId8"/>
-    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId9"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId10"/>
-    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId11"/>
-    <sheet name="accountCreation++" sheetId="39" r:id="rId12"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId13"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId14"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId15"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId16"/>
-    <sheet name="Russels" sheetId="26" r:id="rId17"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId18"/>
-    <sheet name="Login++" sheetId="25" r:id="rId19"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId20"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId21"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId22"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId23"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId24"/>
+    <sheet name="adminUserUpdate++" sheetId="50" r:id="rId7"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId8"/>
+    <sheet name="ic_login++" sheetId="44" r:id="rId9"/>
+    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId10"/>
+    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId11"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId12"/>
+    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId13"/>
+    <sheet name="accountCreation++" sheetId="39" r:id="rId14"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId15"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId16"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId17"/>
+    <sheet name="Russels" sheetId="26" r:id="rId18"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId19"/>
+    <sheet name="Login++" sheetId="25" r:id="rId20"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId21"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId22"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId23"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId24"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId25"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="299">
   <si>
     <t>testSuitID</t>
   </si>
@@ -466,12 +467,6 @@
     <t>SAID</t>
   </si>
   <si>
-    <t>Backend_Lastname</t>
-  </si>
-  <si>
-    <t>Backend_Fisrtname</t>
-  </si>
-  <si>
     <t>DelayforElements</t>
   </si>
   <si>
@@ -850,31 +845,97 @@
     <t>16</t>
   </si>
   <si>
+    <t>Customer Update</t>
+  </si>
+  <si>
+    <t>SapCustomerCreation</t>
+  </si>
+  <si>
+    <t>SapCustomerUpdate</t>
+  </si>
+  <si>
+    <t>Customer Creation</t>
+  </si>
+  <si>
+    <t>Broan</t>
+  </si>
+  <si>
+    <t>7902211821087</t>
+  </si>
+  <si>
+    <t>Jessica</t>
+  </si>
+  <si>
     <t>ICUpdateUser</t>
   </si>
   <si>
-    <t>fake570945622889867@automationjdg.co.za</t>
-  </si>
-  <si>
-    <t>Customer Update</t>
-  </si>
-  <si>
-    <t>SapCustomerCreation</t>
-  </si>
-  <si>
-    <t>SapCustomerUpdate</t>
-  </si>
-  <si>
-    <t>Customer Creation</t>
-  </si>
-  <si>
-    <t>Broan</t>
-  </si>
-  <si>
-    <t>7902211821087</t>
-  </si>
-  <si>
-    <t>Jessica</t>
+    <t>SapCustomerUpdateBackend</t>
+  </si>
+  <si>
+    <t>adminFirstName_output</t>
+  </si>
+  <si>
+    <t>adminLastName_output</t>
+  </si>
+  <si>
+    <t>adminTaxVat_output</t>
+  </si>
+  <si>
+    <t>adminEmail_output</t>
+  </si>
+  <si>
+    <t>adminBilling_streetAddress_output</t>
+  </si>
+  <si>
+    <t>SapCustomerCreationBackend</t>
+  </si>
+  <si>
+    <t>Customer Creation Magento Admin</t>
+  </si>
+  <si>
+    <t>Customer Update Magento Admin</t>
+  </si>
+  <si>
+    <t>8706149754081</t>
+  </si>
+  <si>
+    <t>40 Pritchard Street</t>
+  </si>
+  <si>
+    <t>0670441101</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>adminUserUpdate</t>
+  </si>
+  <si>
+    <t>41 Pritchard Street</t>
+  </si>
+  <si>
+    <t>0670441102</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>emailAddress_input</t>
+  </si>
+  <si>
+    <t>2575Updated3585Updated8931Updatedfake567@automationjdg.co.za</t>
+  </si>
+  <si>
+    <t>BackendFirstname</t>
+  </si>
+  <si>
+    <t>BackendLastname</t>
+  </si>
+  <si>
+    <t>original2Ic@automationjdg.co.za</t>
+  </si>
+  <si>
+    <t>DB_connection_master</t>
   </si>
 </sst>
 </file>
@@ -1579,6 +1640,279 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="5" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.1796875" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="9">
+        <v>15</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E2" s="9">
+        <v>300</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="9">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="9">
+        <v>500</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="9">
+        <v>15</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E4" s="9">
+        <v>100</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="9">
+        <v>15</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E5" s="9">
+        <v>400</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="9">
+        <v>15</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E6" s="9">
+        <v>350</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="48.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1644,7 +1978,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1">
@@ -1663,12 +1997,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -1695,16 +2029,16 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>141</v>
@@ -1713,13 +2047,13 @@
         <v>128</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1730,10 +2064,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>295</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>142</v>
+        <v>296</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>137</v>
@@ -1751,29 +2085,89 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J3" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J4" s="1">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I4" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"Main Website,Incredible Connection"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{00000000-0002-0000-0600-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>"SAID,Passport"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" display="TestAutomation2@gmail.com" xr:uid="{DA5EBA3A-A6C4-4272-B9AE-00C4F9FF6FB5}"/>
+    <hyperlink ref="E4" r:id="rId3" display="TestAutomation2@gmail.com" xr:uid="{BA54DFE0-8598-4662-B188-5760F87BAB89}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -2283,10 +2677,10 @@
         <v>118</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>137</v>
@@ -2298,7 +2692,7 @@
         <v>126</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J9" s="1">
         <v>222223081</v>
@@ -2313,7 +2707,7 @@
         <v>101</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>99</v>
@@ -2328,21 +2722,139 @@
         <v>99</v>
       </c>
       <c r="S9" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="1">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J10" s="1">
+        <v>222223082</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="1">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J11" s="1">
+        <v>222223083</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S11" s="1" t="s">
         <v>99</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K9" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K11" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I9 O2:S9" xr:uid="{00000000-0002-0000-0700-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11 O2:S11" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M9" xr:uid="{00000000-0002-0000-0700-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11" xr:uid="{00000000-0002-0000-0700-000002000000}">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L9" xr:uid="{00000000-0002-0000-0700-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L11" xr:uid="{00000000-0002-0000-0700-000003000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2351,211 +2863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>225505</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>225505</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>225505</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>225505</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>225505</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>225505</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1">
-        <v>225505</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>225505</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1">
-        <v>225505</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1">
-        <v>15</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1">
-        <v>225505</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1">
-        <v>16</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1">
-        <v>225504</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1">
-        <v>17</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>225504</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2583,7 +2891,7 @@
         <v>122</v>
       </c>
       <c r="D1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>121</v>
@@ -2636,7 +2944,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -2728,7 +3036,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -2760,10 +3068,10 @@
         <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1">
@@ -2774,10 +3082,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E2" s="1">
         <v>2</v>
@@ -2794,10 +3102,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -2814,13 +3122,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1">
@@ -2831,13 +3139,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2848,13 +3156,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2865,10 +3173,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2879,7 +3187,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2890,7 +3198,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2901,7 +3209,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2912,7 +3220,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2923,7 +3231,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2934,7 +3242,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2945,7 +3253,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2956,7 +3264,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2967,7 +3275,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2978,7 +3286,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2989,7 +3297,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2998,7 +3306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -3103,12 +3411,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3292,7 +3600,7 @@
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>91</v>
@@ -3328,18 +3636,18 @@
         <v>77</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>72</v>
@@ -3348,7 +3656,7 @@
         <v>73</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>79</v>
@@ -3363,13 +3671,95 @@
         <v>2001</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>77</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="5" customFormat="1">
+      <c r="A7" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" s="5">
+        <v>2002</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="5" customFormat="1">
+      <c r="A8" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" s="5">
+        <v>2003</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3380,222 +3770,20 @@
     <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0D00-000002000000}"/>
     <hyperlink ref="L5" r:id="rId4" xr:uid="{00000000-0004-0000-0D00-000003000000}"/>
     <hyperlink ref="L6" r:id="rId5" xr:uid="{D28DE565-312A-43A7-A8DC-0358A4A221C9}"/>
+    <hyperlink ref="L7" r:id="rId6" xr:uid="{2CC2B3AA-DC58-4653-834F-0B948250005A}"/>
+    <hyperlink ref="L8" r:id="rId7" xr:uid="{CD398B9E-99AC-45FD-9C08-34E835080C53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="9.1796875" style="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1">
-      <c r="A8" s="1">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1">
-      <c r="A9" s="1">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="1" customFormat="1">
-      <c r="A11" s="1">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1">
-      <c r="A12" s="1">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="1" customFormat="1">
-      <c r="A13" s="1">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3840,22 +4028,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>150</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>152</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>90</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -3863,16 +4051,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>31</v>
@@ -3887,7 +4075,7 @@
         <v>32</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>119</v>
@@ -3898,20 +4086,20 @@
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>32</v>
@@ -3937,28 +4125,30 @@
         <v>16</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>90</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="J12" s="9"/>
+        <v>263</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>298</v>
+      </c>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
@@ -3970,15 +4160,17 @@
         <v>17</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="9"/>
       <c r="F13" s="9" t="s">
         <v>116</v>
       </c>
@@ -3986,15 +4178,102 @@
         <v>90</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="I13" s="9"/>
+        <v>263</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>298</v>
+      </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="9">
+        <v>18</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="9">
+        <v>19</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
@@ -4018,6 +4297,210 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -4146,7 +4629,7 @@
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
@@ -4176,7 +4659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -4280,7 +4763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -4384,7 +4867,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -4488,7 +4971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -4597,7 +5080,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4612,16 +5095,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>85</v>
@@ -4632,13 +5115,13 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="D2" s="1">
         <v>30215</v>
@@ -4647,37 +5130,37 @@
         <v>225505</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -4691,16 +5174,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EAF6A5-118F-420D-9E27-9E4187D54643}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
@@ -4713,10 +5196,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4727,10 +5210,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4741,10 +5224,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4755,10 +5238,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4769,10 +5252,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4783,16 +5266,44 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6" xr:uid="{67E12FF2-6850-4102-99AC-26F4FD2C43B1}">
-      <formula1>"Customer Creation, Customer Update"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{7AAC201A-8D7A-4794-936C-C9740DEC397F}">
+      <formula1>"Customer Creation, Customer Update,Customer Creation Magento Admin, Customer Update Magento Admin"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4804,7 +5315,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.54296875" defaultRowHeight="23.25" customHeight="1"/>
@@ -4824,10 +5335,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="23.25" customHeight="1">
@@ -4838,10 +5349,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -4851,10 +5362,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06676BC0-44D6-4FA2-911F-F0A0491104F9}">
-  <dimension ref="A1:AB13"/>
+  <dimension ref="A1:AB16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4873,9 +5384,13 @@
     <col min="12" max="12" width="18.26953125" style="1" customWidth="1"/>
     <col min="13" max="13" width="15.81640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.08984375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.7265625" style="1"/>
+    <col min="15" max="15" width="20.90625" style="1" customWidth="1"/>
     <col min="16" max="16" width="21.7265625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.7265625" style="1"/>
+    <col min="17" max="17" width="13.36328125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="19.08984375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="22.1796875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="22.7265625" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="58">
@@ -4889,82 +5404,82 @@
         <v>61</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>114</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="H1" s="21" t="s">
         <v>224</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>226</v>
       </c>
       <c r="I1" s="21" t="s">
         <v>69</v>
       </c>
       <c r="J1" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="L1" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="Q1" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="S1" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="T1" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="U1" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="V1" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="W1" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="X1" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="Y1" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="Z1" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="AA1" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="Z1" s="21" t="s">
+      <c r="AB1" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="AA1" s="21" t="s">
-        <v>244</v>
-      </c>
-      <c r="AB1" s="21" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" ht="29">
+    </row>
+    <row r="2" spans="1:28">
       <c r="A2" s="21">
         <v>3</v>
       </c>
@@ -4999,9 +5514,7 @@
       </c>
       <c r="O2" s="21"/>
       <c r="P2" s="21"/>
-      <c r="Q2" s="21" t="s">
-        <v>246</v>
-      </c>
+      <c r="Q2" s="21"/>
       <c r="R2" s="21"/>
       <c r="S2" s="21"/>
       <c r="T2" s="21"/>
@@ -5055,9 +5568,7 @@
       </c>
       <c r="O3" s="21"/>
       <c r="P3" s="21"/>
-      <c r="Q3" s="21" t="s">
-        <v>246</v>
-      </c>
+      <c r="Q3" s="21"/>
       <c r="R3" s="21"/>
       <c r="S3" s="21"/>
       <c r="T3" s="21"/>
@@ -5070,7 +5581,7 @@
       <c r="W3" s="21"/>
       <c r="X3" s="21"/>
       <c r="Y3" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Z3" s="21"/>
       <c r="AA3" s="21"/>
@@ -5111,9 +5622,7 @@
       </c>
       <c r="O4" s="21"/>
       <c r="P4" s="21"/>
-      <c r="Q4" s="21" t="s">
-        <v>246</v>
-      </c>
+      <c r="Q4" s="21"/>
       <c r="R4" s="21"/>
       <c r="S4" s="21"/>
       <c r="T4" s="21"/>
@@ -5126,7 +5635,7 @@
       <c r="W4" s="21"/>
       <c r="X4" s="21"/>
       <c r="Y4" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Z4" s="21"/>
       <c r="AA4" s="21"/>
@@ -5167,9 +5676,7 @@
       </c>
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
-      <c r="Q5" s="21" t="s">
-        <v>246</v>
-      </c>
+      <c r="Q5" s="21"/>
       <c r="R5" s="21"/>
       <c r="S5" s="21"/>
       <c r="T5" s="21"/>
@@ -5182,7 +5689,7 @@
       <c r="W5" s="21"/>
       <c r="X5" s="21"/>
       <c r="Y5" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Z5" s="21"/>
       <c r="AA5" s="21"/>
@@ -5223,9 +5730,7 @@
       </c>
       <c r="O6" s="21"/>
       <c r="P6" s="21"/>
-      <c r="Q6" s="21" t="s">
-        <v>246</v>
-      </c>
+      <c r="Q6" s="21"/>
       <c r="R6" s="21"/>
       <c r="S6" s="21"/>
       <c r="T6" s="21"/>
@@ -5238,7 +5743,7 @@
       <c r="W6" s="21"/>
       <c r="X6" s="21"/>
       <c r="Y6" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Z6" s="21"/>
       <c r="AA6" s="21"/>
@@ -5279,9 +5784,7 @@
       </c>
       <c r="O7" s="21"/>
       <c r="P7" s="21"/>
-      <c r="Q7" s="21" t="s">
-        <v>246</v>
-      </c>
+      <c r="Q7" s="21"/>
       <c r="R7" s="21"/>
       <c r="S7" s="21"/>
       <c r="T7" s="21"/>
@@ -5294,7 +5797,7 @@
       <c r="W7" s="21"/>
       <c r="X7" s="21"/>
       <c r="Y7" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Z7" s="21"/>
       <c r="AA7" s="21"/>
@@ -5335,9 +5838,7 @@
       </c>
       <c r="O8" s="21"/>
       <c r="P8" s="21"/>
-      <c r="Q8" s="21" t="s">
-        <v>246</v>
-      </c>
+      <c r="Q8" s="21"/>
       <c r="R8" s="21"/>
       <c r="S8" s="21"/>
       <c r="T8" s="21"/>
@@ -5350,7 +5851,7 @@
       <c r="W8" s="21"/>
       <c r="X8" s="21"/>
       <c r="Y8" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Z8" s="21"/>
       <c r="AA8" s="21"/>
@@ -5391,9 +5892,7 @@
       </c>
       <c r="O9" s="21"/>
       <c r="P9" s="21"/>
-      <c r="Q9" s="21" t="s">
-        <v>246</v>
-      </c>
+      <c r="Q9" s="21"/>
       <c r="R9" s="21"/>
       <c r="S9" s="21"/>
       <c r="T9" s="21"/>
@@ -5406,7 +5905,7 @@
       <c r="W9" s="21"/>
       <c r="X9" s="21"/>
       <c r="Y9" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Z9" s="21"/>
       <c r="AA9" s="21"/>
@@ -5447,9 +5946,7 @@
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="21"/>
-      <c r="Q10" s="21" t="s">
-        <v>246</v>
-      </c>
+      <c r="Q10" s="21"/>
       <c r="R10" s="21"/>
       <c r="S10" s="21"/>
       <c r="T10" s="21"/>
@@ -5462,7 +5959,7 @@
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
       <c r="Y10" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Z10" s="21"/>
       <c r="AA10" s="21"/>
@@ -5503,9 +6000,7 @@
       </c>
       <c r="O11" s="21"/>
       <c r="P11" s="21"/>
-      <c r="Q11" s="21" t="s">
-        <v>246</v>
-      </c>
+      <c r="Q11" s="21"/>
       <c r="R11" s="21"/>
       <c r="S11" s="21"/>
       <c r="T11" s="21"/>
@@ -5518,7 +6013,7 @@
       <c r="W11" s="21"/>
       <c r="X11" s="21"/>
       <c r="Y11" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Z11" s="21"/>
       <c r="AA11" s="21"/>
@@ -5559,9 +6054,7 @@
       </c>
       <c r="O12" s="21"/>
       <c r="P12" s="21"/>
-      <c r="Q12" s="21" t="s">
-        <v>246</v>
-      </c>
+      <c r="Q12" s="21"/>
       <c r="R12" s="21"/>
       <c r="S12" s="21"/>
       <c r="T12" s="21"/>
@@ -5574,7 +6067,7 @@
       <c r="W12" s="21"/>
       <c r="X12" s="21"/>
       <c r="Y12" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Z12" s="21"/>
       <c r="AA12" s="21"/>
@@ -5596,11 +6089,11 @@
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" s="21"/>
       <c r="I13" s="21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J13" s="21"/>
       <c r="K13" s="21" t="s">
@@ -5611,13 +6104,11 @@
         <v>9</v>
       </c>
       <c r="N13" s="21" t="s">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="O13" s="21"/>
       <c r="P13" s="21"/>
-      <c r="Q13" s="21" t="s">
-        <v>246</v>
-      </c>
+      <c r="Q13" s="21"/>
       <c r="R13" s="21"/>
       <c r="S13" s="21"/>
       <c r="T13" s="21"/>
@@ -5630,11 +6121,173 @@
       <c r="W13" s="21"/>
       <c r="X13" s="21"/>
       <c r="Y13" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Z13" s="21"/>
       <c r="AA13" s="21"/>
       <c r="AB13" s="21"/>
+    </row>
+    <row r="14" spans="1:28" ht="29">
+      <c r="A14" s="21">
+        <v>19</v>
+      </c>
+      <c r="B14" s="21">
+        <v>1</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="V14" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="W14" s="21"/>
+      <c r="X14" s="21"/>
+      <c r="Y14" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z14" s="21"/>
+      <c r="AA14" s="21"/>
+      <c r="AB14" s="21"/>
+    </row>
+    <row r="15" spans="1:28" ht="29">
+      <c r="A15" s="21">
+        <v>18</v>
+      </c>
+      <c r="B15" s="21">
+        <v>1</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="V15" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="W15" s="21"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z15" s="21"/>
+      <c r="AA15" s="21"/>
+      <c r="AB15" s="21"/>
+    </row>
+    <row r="16" spans="1:28" ht="29">
+      <c r="A16" s="21">
+        <v>15</v>
+      </c>
+      <c r="B16" s="21">
+        <v>1</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="V16" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="W16" s="21"/>
+      <c r="X16" s="21"/>
+      <c r="Y16" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z16" s="21"/>
+      <c r="AA16" s="21"/>
+      <c r="AB16" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5642,11 +6295,636 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65EB4B98-E5C5-4A51-A353-3C573AAFE2D2}">
+  <dimension ref="A1:AA8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="3" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="21.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="21.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="1"/>
+    <col min="8" max="8" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" style="1"/>
+    <col min="10" max="10" width="25.6328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" style="1"/>
+    <col min="16" max="16" width="25.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.453125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8.7265625" style="1"/>
+    <col min="19" max="19" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="26" width="8.7265625" style="1"/>
+    <col min="27" max="27" width="13.453125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="17.08984375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11.54296875" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" s="1">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" s="1">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" s="1">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" s="1">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" s="1">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" s="1">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P12 X3:X12" xr:uid="{B0A7B443-6DB9-4C76-AE05-20C4BAEA5267}">
+      <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12 L2:N12 E2:E12 G2:G12 C2:C12 T2:V12" xr:uid="{49306ACA-D47A-45D5-A248-AE5CF6AA65C4}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="J5" r:id="rId1" xr:uid="{CB312BC1-5B63-46C6-B8C5-892434A66A94}"/>
+    <hyperlink ref="J6:J8" r:id="rId2" display="original2Ic@automationjdg.co.za" xr:uid="{3327310A-17C6-4267-BC1A-256340654B5F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>225505</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>225505</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>225505</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>225505</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>225505</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>225505</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>225505</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>225505</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>225505</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>225505</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>225504</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>225504</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>225504</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>225504</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -5678,11 +6956,11 @@
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>220</v>
+      <c r="C2" s="20" t="s">
+        <v>218</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5693,7 +6971,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>271</v>
+        <v>294</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>126</v>
@@ -5703,300 +6981,28 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{041402AB-69A1-471C-9606-CFF8B1A19818}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{FD7045F4-1BC8-4D9F-B6B0-E7C72C2DCFDD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="5" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.54296875" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.54296875" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.1796875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="9">
-        <v>15</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="E2" s="9">
-        <v>300</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="9">
-        <v>15</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="E3" s="9">
-        <v>500</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="9">
-        <v>15</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="E4" s="9">
-        <v>100</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="9">
-        <v>15</v>
-      </c>
-      <c r="B5" s="9">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="E5" s="9">
-        <v>400</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="9">
-        <v>15</v>
-      </c>
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="E6" s="9">
-        <v>350</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>218</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" customWidth="1"/>
-    <col min="3" max="3" width="48.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1">
-      <c r="A1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6149,14 +7155,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -6169,6 +7167,14 @@
     <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
BP number added to data map
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDD5862-278E-4F7D-BA09-376B590B745C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1770" windowWidth="15285" windowHeight="7875" firstSheet="13" activeTab="16"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="253">
   <si>
     <t>testSuitID</t>
   </si>
@@ -791,12 +792,18 @@
   </si>
   <si>
     <t>Samsung Toner D105L</t>
+  </si>
+  <si>
+    <t>DB_connection_master</t>
+  </si>
+  <si>
+    <t>BP_Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -914,7 +921,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -945,6 +952,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1057,7 +1066,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1090,9 +1099,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1125,6 +1151,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1300,7 +1343,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1465,7 +1508,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1511,7 +1554,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1607,7 +1650,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1696,15 +1739,15 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>"Main Website,Incredible Connection"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{00000000-0002-0000-0B00-000001000000}">
       <formula1>"SAID,Passport"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1712,7 +1755,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -2158,16 +2201,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K7" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I7 O2:S7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I7 O2:S7" xr:uid="{00000000-0002-0000-0C00-000001000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M7" xr:uid="{00000000-0002-0000-0C00-000002000000}">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L7" xr:uid="{00000000-0002-0000-0C00-000003000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2177,7 +2220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2353,7 +2396,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2434,7 +2477,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2526,10 +2569,10 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -2910,7 +2953,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3015,7 +3058,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3285,11 +3328,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="L4" r:id="rId3"/>
-    <hyperlink ref="L5" r:id="rId4"/>
-    <hyperlink ref="L6" r:id="rId5"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-1200-000001000000}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-1200-000002000000}"/>
+    <hyperlink ref="L5" r:id="rId4" xr:uid="{00000000-0004-0000-1200-000003000000}"/>
+    <hyperlink ref="L6" r:id="rId5" xr:uid="{00000000-0004-0000-1200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
@@ -3297,11 +3340,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3700,6 +3743,50 @@
       </c>
       <c r="J13" s="15" t="s">
         <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -3724,7 +3811,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3928,7 +4015,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4113,7 +4200,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4217,7 +4304,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4321,7 +4408,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4425,7 +4512,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="L14" workbookViewId="0">
@@ -4529,7 +4616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4593,7 +4680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4676,7 +4763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4763,7 +4850,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -4771,11 +4858,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4784,10 +4871,11 @@
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="5" max="5" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -4800,8 +4888,11 @@
       <c r="D1" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4815,7 +4906,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1">
+    <row r="3" spans="1:5" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>10</v>
       </c>
@@ -4835,7 +4926,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4944,7 +5035,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5042,7 +5133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5162,10 +5253,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="G2" r:id="rId2"/>
-    <hyperlink ref="I3" r:id="rId3"/>
-    <hyperlink ref="G3" r:id="rId4"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="I3" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5181,6 +5272,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5329,15 +5429,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
@@ -5347,6 +5438,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5363,21 +5471,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
End to End working
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2172AA88-385B-46FE-9392-A314EDE6C35F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="giftCardReport++" sheetId="54" r:id="rId1"/>
@@ -13,42 +14,44 @@
     <sheet name="SapCustomer++" sheetId="50" r:id="rId4"/>
     <sheet name="Suites" sheetId="22" r:id="rId5"/>
     <sheet name="IC" sheetId="23" r:id="rId6"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId7"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId8"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId9"/>
-    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId10"/>
-    <sheet name="SAP_OrderRelated++" sheetId="46" r:id="rId11"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId12"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId13"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId14"/>
-    <sheet name="ic_RetriveOrderID++" sheetId="53" r:id="rId15"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId16"/>
-    <sheet name="icRedeemGiftCard++" sheetId="48" r:id="rId17"/>
-    <sheet name="VeriyGiftcardUsableity++" sheetId="49" r:id="rId18"/>
-    <sheet name="ic_login++" sheetId="44" r:id="rId19"/>
-    <sheet name="DB_connection_master++" sheetId="47" r:id="rId20"/>
-    <sheet name="icGiftCardVerificationSender++" sheetId="45" r:id="rId21"/>
-    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId22"/>
-    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId23"/>
-    <sheet name="accountCreation++" sheetId="39" r:id="rId24"/>
-    <sheet name="Russels" sheetId="26" r:id="rId25"/>
-    <sheet name="Login++" sheetId="25" r:id="rId26"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId27"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId28"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId29"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId30"/>
+    <sheet name="CreditStatusVerification++" sheetId="56" r:id="rId7"/>
+    <sheet name="CreditApp_NavigateFilter++" sheetId="55" r:id="rId8"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId9"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId10"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId11"/>
+    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId12"/>
+    <sheet name="SAP_OrderRelated++" sheetId="46" r:id="rId13"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId14"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId15"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId16"/>
+    <sheet name="ic_RetriveOrderID++" sheetId="53" r:id="rId17"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId18"/>
+    <sheet name="icRedeemGiftCard++" sheetId="48" r:id="rId19"/>
+    <sheet name="VeriyGiftcardUsableity++" sheetId="49" r:id="rId20"/>
+    <sheet name="ic_login++" sheetId="44" r:id="rId21"/>
+    <sheet name="DB_connection_master++" sheetId="47" r:id="rId22"/>
+    <sheet name="icGiftCardVerificationSender++" sheetId="45" r:id="rId23"/>
+    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId24"/>
+    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId25"/>
+    <sheet name="accountCreation++" sheetId="39" r:id="rId26"/>
+    <sheet name="Russels" sheetId="26" r:id="rId27"/>
+    <sheet name="Login++" sheetId="25" r:id="rId28"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId29"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId30"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId31"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId32"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -65,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -87,12 +90,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -110,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="366">
   <si>
     <t>testSuitID</t>
   </si>
@@ -1183,12 +1186,45 @@
   </si>
   <si>
     <t>Canon 737 Blk Toner</t>
+  </si>
+  <si>
+    <t>Credit application-verification Magento admin</t>
+  </si>
+  <si>
+    <t>CreditApp_NavigateFilter</t>
+  </si>
+  <si>
+    <t>TomasCardosoLima@dayrep.com</t>
+  </si>
+  <si>
+    <t>EmailIdtoFilter</t>
+  </si>
+  <si>
+    <t>Credit app verification in magento admin</t>
+  </si>
+  <si>
+    <t>Access#3</t>
+  </si>
+  <si>
+    <t>CreditStatusVerification</t>
+  </si>
+  <si>
+    <t>Final_ExpectedStatus</t>
+  </si>
+  <si>
+    <t>TimeOut_Inseconds</t>
+  </si>
+  <si>
+    <t>WaitTime</t>
+  </si>
+  <si>
+    <t>Declined</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -1284,7 +1320,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1344,12 +1380,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1494,6 +1539,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1504,6 +1552,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1552,7 +1603,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1585,9 +1636,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1620,6 +1688,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1795,7 +1880,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1914,7 +1999,636 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="33.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30">
+      <c r="A2" s="19">
+        <v>26</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="C2" s="20">
+        <v>1</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="45">
+      <c r="A3" s="19">
+        <v>27</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>329</v>
+      </c>
+      <c r="C3" s="20">
+        <v>1</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="45">
+      <c r="A4" s="19">
+        <v>28</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="C4" s="20">
+        <v>1</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30">
+      <c r="A5" s="19">
+        <v>29</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="C5" s="20">
+        <v>1</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30">
+      <c r="A6" s="19">
+        <v>30</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="C6" s="20">
+        <v>1</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30">
+      <c r="A7" s="20">
+        <v>31</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7" s="20">
+        <v>1</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="20">
+        <v>32</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="C8" s="20">
+        <v>1</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="42">
+        <v>33</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="C9" s="20">
+        <v>1</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="42">
+        <v>34</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="C10" s="20">
+        <v>1</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="42">
+        <v>35</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="C11" s="43">
+        <v>1</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="42">
+        <v>36</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="C12" s="43">
+        <v>1</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>325</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0700-000000000000}">
+      <formula1>"payUcreditcard,Cash_Deposits"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="5" customFormat="1">
+      <c r="A1" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="30">
+      <c r="A2" s="19">
+        <v>26</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>313</v>
+      </c>
+      <c r="C2" s="30">
+        <v>1</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="30">
+        <v>2000</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="5" customFormat="1" ht="45">
+      <c r="A3" s="19">
+        <v>27</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>329</v>
+      </c>
+      <c r="C3" s="30">
+        <v>1</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="K3" s="30">
+        <v>2000</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="5" customFormat="1" ht="45">
+      <c r="A4" s="19">
+        <v>28</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="C4" s="30">
+        <v>1</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="30">
+        <v>2000</v>
+      </c>
+      <c r="L4" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="5" customFormat="1" ht="30">
+      <c r="A5" s="19">
+        <v>29</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>314</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="K5" s="30">
+        <v>2000</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" s="32" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="5" customFormat="1" ht="30">
+      <c r="A6" s="19">
+        <v>30</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>315</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="30">
+        <v>2000</v>
+      </c>
+      <c r="L6" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="N6" s="32" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="5" customFormat="1" ht="30">
+      <c r="A7" s="19">
+        <v>31</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="K7" s="30">
+        <v>2000</v>
+      </c>
+      <c r="L7" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" s="32" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="5" customFormat="1" ht="30">
+      <c r="A8" s="19">
+        <v>32</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="K8" s="30">
+        <v>2000</v>
+      </c>
+      <c r="L8" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="N8" s="32" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="30">
+      <c r="A9" s="42">
+        <v>35</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9" s="30">
+        <v>2000</v>
+      </c>
+      <c r="L9" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="M4" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="M5" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="M8" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="M6" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="M7" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="M9" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2145,23 +2859,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="H2" r:id="rId2"/>
-    <hyperlink ref="J3" r:id="rId3"/>
-    <hyperlink ref="H3" r:id="rId4"/>
-    <hyperlink ref="J4" r:id="rId5"/>
-    <hyperlink ref="H4" r:id="rId6"/>
-    <hyperlink ref="J5" r:id="rId7"/>
-    <hyperlink ref="H5" r:id="rId8"/>
-    <hyperlink ref="J6" r:id="rId9"/>
-    <hyperlink ref="H6" r:id="rId10"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="J3" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="H3" r:id="rId4" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="J4" r:id="rId5" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="H4" r:id="rId6" xr:uid="{00000000-0004-0000-0900-000005000000}"/>
+    <hyperlink ref="J5" r:id="rId7" xr:uid="{00000000-0004-0000-0900-000006000000}"/>
+    <hyperlink ref="H5" r:id="rId8" xr:uid="{00000000-0004-0000-0900-000007000000}"/>
+    <hyperlink ref="J6" r:id="rId9" xr:uid="{00000000-0004-0000-0900-000008000000}"/>
+    <hyperlink ref="H6" r:id="rId10" xr:uid="{00000000-0004-0000-0900-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2369,8 +3083,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2590,8 +3304,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -2839,15 +3553,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3131,7 +3845,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:5">
       <c r="A17" s="19">
         <v>16</v>
       </c>
@@ -3148,7 +3862,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:5">
       <c r="A18" s="19">
         <v>17</v>
       </c>
@@ -3165,7 +3879,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:5">
       <c r="A19" s="19">
         <v>18</v>
       </c>
@@ -3182,7 +3896,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:5">
       <c r="A20" s="19">
         <v>19</v>
       </c>
@@ -3199,7 +3913,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:5">
       <c r="A21" s="19">
         <v>20</v>
       </c>
@@ -3216,7 +3930,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30">
+    <row r="22" spans="1:5" ht="30">
       <c r="A22" s="19">
         <v>26</v>
       </c>
@@ -3233,7 +3947,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30">
+    <row r="23" spans="1:5" ht="30">
       <c r="A23" s="19">
         <v>27</v>
       </c>
@@ -3250,7 +3964,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="19">
         <v>28</v>
       </c>
@@ -3267,7 +3981,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:5">
       <c r="A25" s="19">
         <v>29</v>
       </c>
@@ -3284,7 +3998,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="30">
+    <row r="26" spans="1:5" ht="30">
       <c r="A26" s="19">
         <v>30</v>
       </c>
@@ -3301,7 +4015,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:5" s="35" customFormat="1">
       <c r="A27" s="19">
         <v>31</v>
       </c>
@@ -3318,11 +4032,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="42">
+    <row r="28" spans="1:5" s="35" customFormat="1">
+      <c r="A28" s="19">
         <v>32</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="19" t="s">
         <v>334</v>
       </c>
       <c r="C28" s="19">
@@ -3335,11 +4049,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="42">
+    <row r="29" spans="1:5" s="35" customFormat="1">
+      <c r="A29" s="19">
         <v>33</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="19" t="s">
         <v>335</v>
       </c>
       <c r="C29" s="19">
@@ -3352,11 +4066,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="42">
+    <row r="30" spans="1:5" s="35" customFormat="1">
+      <c r="A30" s="19">
         <v>34</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="19" t="s">
         <v>336</v>
       </c>
       <c r="C30" s="19">
@@ -3368,13 +4082,12 @@
       <c r="E30" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="F30" s="35"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="42">
+    </row>
+    <row r="31" spans="1:5" s="35" customFormat="1">
+      <c r="A31" s="19">
         <v>37</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="19" t="s">
         <v>339</v>
       </c>
       <c r="C31" s="19">
@@ -3387,11 +4100,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="42">
+    <row r="32" spans="1:5" s="35" customFormat="1">
+      <c r="A32" s="19">
         <v>38</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="19" t="s">
         <v>340</v>
       </c>
       <c r="C32" s="19">
@@ -3402,6 +4115,23 @@
       </c>
       <c r="E32" s="19" t="s">
         <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="35" customFormat="1">
+      <c r="A33" s="19">
+        <v>42</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="C33" s="19">
+        <v>1</v>
+      </c>
+      <c r="D33" s="19">
+        <v>225564</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -3410,8 +4140,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3575,8 +4305,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4165,8 +4895,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4268,324 +4998,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>16</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="F2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1">
-      <c r="A3" s="1">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>100</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="38.140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="19">
-        <v>15</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>262</v>
-      </c>
-      <c r="C2" s="19">
-        <v>1</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="19">
-        <v>16</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>263</v>
-      </c>
-      <c r="C3" s="19">
-        <v>1</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="19">
-        <v>17</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>264</v>
-      </c>
-      <c r="C4" s="19">
-        <v>1</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="19">
-        <v>18</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>265</v>
-      </c>
-      <c r="C5" s="19">
-        <v>1</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="12" customFormat="1">
-      <c r="A6" s="19">
-        <v>19</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>266</v>
-      </c>
-      <c r="C6" s="19">
-        <v>1</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="19">
-        <v>20</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>312</v>
-      </c>
-      <c r="C7" s="19">
-        <v>1</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="19">
-        <v>33</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>335</v>
-      </c>
-      <c r="C8" s="19">
-        <v>1</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="19">
-        <v>36</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>338</v>
-      </c>
-      <c r="C9" s="19">
-        <v>1</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="19"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="19"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="19"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="19"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="19"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="19"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="19"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E6" r:id="rId2"/>
-    <hyperlink ref="E7" r:id="rId3"/>
-    <hyperlink ref="E8" r:id="rId4"/>
-    <hyperlink ref="E9" r:id="rId5"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5014,25 +5428,341 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:W10 I2:I10 K2:K10 M2:O10 G2:G10 E2:E10 F5:F7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:W10 I2:I10 K2:K10 M2:O10 G2:G10 E2:E10 F5:F7" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
-    <hyperlink ref="D6:D7" r:id="rId2" display="original2Ic@automationjdg.co.za"/>
-    <hyperlink ref="D7" r:id="rId3"/>
-    <hyperlink ref="D2:D4" r:id="rId4" display="original2Ic@automationjdg.co.za"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D6:D7" r:id="rId2" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D2:D4" r:id="rId4" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>100</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="38.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="19">
+        <v>15</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" s="19">
+        <v>1</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="19">
+        <v>16</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="C3" s="19">
+        <v>1</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="19">
+        <v>17</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="C4" s="19">
+        <v>1</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="19">
+        <v>18</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="19">
+        <v>1</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="12" customFormat="1">
+      <c r="A6" s="19">
+        <v>19</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="C6" s="19">
+        <v>1</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="19">
+        <v>20</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" s="19">
+        <v>1</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="19">
+        <v>33</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="C8" s="19">
+        <v>1</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="19">
+        <v>36</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="19"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="19"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="19"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="19"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="19"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="19"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="19"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{00000000-0004-0000-1200-000001000000}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{00000000-0004-0000-1200-000002000000}"/>
+    <hyperlink ref="E8" r:id="rId4" xr:uid="{00000000-0004-0000-1200-000003000000}"/>
+    <hyperlink ref="E9" r:id="rId5" xr:uid="{00000000-0004-0000-1200-000004000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5136,15 +5866,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5241,8 +5971,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5287,8 +6017,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5578,17 +6308,17 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{00000000-0002-0000-1600-000000000000}">
       <formula1>"Main Website,Incredible Connection"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G4 F5:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G4 F5:F1048576" xr:uid="{00000000-0002-0000-1600-000001000000}">
       <formula1>"SAID,Passport"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com"/>
-    <hyperlink ref="F3" r:id="rId2" display="TestAutomation2@gmail.com"/>
-    <hyperlink ref="F4" r:id="rId3" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-1600-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-1600-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -5596,8 +6326,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6281,16 +7011,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K11" xr:uid="{00000000-0002-0000-1700-000000000000}">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11 O2:S11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11 O2:S11" xr:uid="{00000000-0002-0000-1700-000001000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11" xr:uid="{00000000-0002-0000-1700-000002000000}">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L11" xr:uid="{00000000-0002-0000-1700-000003000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6299,8 +7029,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6404,8 +7134,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6608,8 +7338,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6712,216 +7442,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -8303,7 +8825,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:O1048576 L2:L1048576 J2:J1048576 H2:H1048576 F2:F1048576 D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:O1048576 L2:L1048576 J2:J1048576 H2:H1048576 F2:F1048576 D2:D1048576" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8312,7 +8834,215 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="L14" workbookViewId="0">
@@ -8416,7 +9146,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8812,7 +9542,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Guest Customer Creation, Customer Creation, Customer Update,Customer Creation Magento Admin, Customer Update Magento Admin"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8821,7 +9551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -8986,14 +9716,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F27" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="D33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9351,7 +10078,7 @@
       <c r="D10" s="48" t="s">
         <v>248</v>
       </c>
-      <c r="E10" s="47" t="s">
+      <c r="E10" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="47" t="s">
@@ -9387,7 +10114,7 @@
       <c r="D11" s="48" t="s">
         <v>249</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="47" t="s">
@@ -9423,7 +10150,7 @@
       <c r="D12" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="E12" s="47" t="s">
+      <c r="E12" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="47" t="s">
@@ -9459,7 +10186,7 @@
       <c r="D13" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="47" t="s">
@@ -9495,7 +10222,7 @@
       <c r="D14" s="48" t="s">
         <v>252</v>
       </c>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="47" t="s">
@@ -9531,7 +10258,7 @@
       <c r="D15" s="48" t="s">
         <v>252</v>
       </c>
-      <c r="E15" s="47" t="s">
+      <c r="E15" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="47" t="s">
@@ -9567,7 +10294,7 @@
       <c r="D16" s="48" t="s">
         <v>248</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="47" t="s">
@@ -9605,7 +10332,7 @@
       <c r="D17" s="48" t="s">
         <v>249</v>
       </c>
-      <c r="E17" s="47" t="s">
+      <c r="E17" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="47" t="s">
@@ -9643,7 +10370,7 @@
       <c r="D18" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E18" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="47" t="s">
@@ -9681,7 +10408,7 @@
       <c r="D19" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="E19" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="47" t="s">
@@ -9719,7 +10446,7 @@
       <c r="D20" s="48" t="s">
         <v>252</v>
       </c>
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="47" t="s">
@@ -9757,7 +10484,7 @@
       <c r="D21" s="48" t="s">
         <v>312</v>
       </c>
-      <c r="E21" s="47" t="s">
+      <c r="E21" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="47"/>
@@ -9793,7 +10520,7 @@
       <c r="D22" s="34" t="s">
         <v>318</v>
       </c>
-      <c r="E22" s="47" t="s">
+      <c r="E22" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="14"/>
@@ -9823,7 +10550,7 @@
       <c r="D23" s="34" t="s">
         <v>318</v>
       </c>
-      <c r="E23" s="47" t="s">
+      <c r="E23" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="14"/>
@@ -9853,7 +10580,7 @@
       <c r="D24" s="34" t="s">
         <v>318</v>
       </c>
-      <c r="E24" s="47" t="s">
+      <c r="E24" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="14"/>
@@ -9883,7 +10610,7 @@
       <c r="D25" s="34" t="s">
         <v>318</v>
       </c>
-      <c r="E25" s="47" t="s">
+      <c r="E25" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F25" s="14"/>
@@ -9913,7 +10640,7 @@
       <c r="D26" s="34" t="s">
         <v>318</v>
       </c>
-      <c r="E26" s="47" t="s">
+      <c r="E26" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="14"/>
@@ -10172,7 +10899,7 @@
         <v>215</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F32" s="47"/>
       <c r="G32" s="49" t="s">
@@ -10492,7 +11219,7 @@
       <c r="D40" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="E40" s="53" t="s">
+      <c r="E40" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F40" s="53" t="s">
@@ -10648,7 +11375,7 @@
       <c r="D44" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="E44" s="55" t="s">
+      <c r="E44" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F44" s="55"/>
@@ -10684,7 +11411,7 @@
       <c r="D45" s="52" t="s">
         <v>238</v>
       </c>
-      <c r="E45" s="55" t="s">
+      <c r="E45" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F45" s="55" t="s">
@@ -10752,7 +11479,7 @@
       <c r="D47" s="52" t="s">
         <v>241</v>
       </c>
-      <c r="E47" s="55" t="s">
+      <c r="E47" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F47" s="55"/>
@@ -10784,7 +11511,7 @@
       <c r="D48" s="48" t="s">
         <v>246</v>
       </c>
-      <c r="E48" s="47" t="s">
+      <c r="E48" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F48" s="47" t="s">
@@ -10852,7 +11579,7 @@
       <c r="D50" s="48" t="s">
         <v>253</v>
       </c>
-      <c r="E50" s="47" t="s">
+      <c r="E50" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F50" s="47" t="s">
@@ -10917,146 +11644,178 @@
       </c>
       <c r="P51" s="14"/>
     </row>
+    <row r="52" spans="1:16">
+      <c r="A52" s="14">
+        <v>42</v>
+      </c>
+      <c r="B52" s="58" t="s">
+        <v>355</v>
+      </c>
+      <c r="C52" s="17"/>
+      <c r="D52" s="59" t="s">
+        <v>355</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H52" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="I52" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="J52" s="55"/>
+      <c r="K52" s="55"/>
+      <c r="L52" s="49"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="49"/>
+      <c r="O52" s="55"/>
+      <c r="P52" s="14"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G49" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="G41" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G42:G43" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="H42" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H43" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="G51" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="I51" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="L51" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="N51" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="I3" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G3" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="H4" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="I4" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G4" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="H5" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="I5" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G5" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="H6" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="I6" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G6" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
-    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
-    <hyperlink ref="I8:I9" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="I7" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G2" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="H2" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="I2" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G10:G14" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="H10" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
-    <hyperlink ref="H11:H14" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
-    <hyperlink ref="G15" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="H15" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
-    <hyperlink ref="G16" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="H16" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
-    <hyperlink ref="I16" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G17" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G18" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G19" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G20" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="H17" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
-    <hyperlink ref="H18" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
-    <hyperlink ref="H19" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
-    <hyperlink ref="H20" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
-    <hyperlink ref="I17" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="I18" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="I19" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="I20" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="H21" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
-    <hyperlink ref="I21" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G27" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H27" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="L27" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="N27" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="G24" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="G25" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="G22" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="G23" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="G26" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="I10:I15" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="J17:J21" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="J16" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="I27" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="J27" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="M27" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="K27" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
-    <hyperlink ref="O27" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="G28" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="G30" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H28" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="H30" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="L28" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="L30" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="N28" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="N30" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="I28" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="I30" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="J28" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="J30" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="M28" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="M30" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="K28" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
-    <hyperlink ref="K30" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
-    <hyperlink ref="O28" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="O30" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="G31" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H31" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="K31" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="M31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="I31" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="L31" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="J31" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
-    <hyperlink ref="N31" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="G29" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H29" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="L29" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="N29" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="I29" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="J29" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="M29" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="K29" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
-    <hyperlink ref="O29" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="G32" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H32" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="L32" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="N32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="I32" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="J32" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="M32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="O32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="P32" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G34" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="H37" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H33" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="I33" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="J33" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="K33" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="L33" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="M33" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="N33" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="G33" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
-    <hyperlink ref="H34" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
-    <hyperlink ref="J34" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="K34" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="L34" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="M34" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="N34" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="O34" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="M35" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="G38" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G39" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="H38" location="'giftCardReport++'!A1" display="giftCardReport"/>
-    <hyperlink ref="H39" location="'giftCardReport++'!A1" display="giftCardReport"/>
-    <hyperlink ref="K32" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="G49" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="G41" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="G42:G43" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="H42" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="H43" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="G51" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="I51" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="L51" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="N51" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="I3" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
+    <hyperlink ref="G3" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
+    <hyperlink ref="H4" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
+    <hyperlink ref="I4" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0500-00000D000000}"/>
+    <hyperlink ref="G4" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0500-00000E000000}"/>
+    <hyperlink ref="H5" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
+    <hyperlink ref="I5" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
+    <hyperlink ref="G5" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0500-000011000000}"/>
+    <hyperlink ref="H6" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000012000000}"/>
+    <hyperlink ref="I6" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0500-000013000000}"/>
+    <hyperlink ref="G6" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0500-000014000000}"/>
+    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000015000000}"/>
+    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000016000000}"/>
+    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0500-000017000000}"/>
+    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0500-000018000000}"/>
+    <hyperlink ref="I8:I9" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0500-000019000000}"/>
+    <hyperlink ref="I7" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0500-00001A000000}"/>
+    <hyperlink ref="G2" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0500-00001B000000}"/>
+    <hyperlink ref="H2" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-00001C000000}"/>
+    <hyperlink ref="I2" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0500-00001D000000}"/>
+    <hyperlink ref="G10:G14" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-00001E000000}"/>
+    <hyperlink ref="H10" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0500-00001F000000}"/>
+    <hyperlink ref="H11:H14" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0500-000020000000}"/>
+    <hyperlink ref="G15" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000021000000}"/>
+    <hyperlink ref="H15" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0500-000022000000}"/>
+    <hyperlink ref="G16" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0500-000023000000}"/>
+    <hyperlink ref="H16" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0500-000024000000}"/>
+    <hyperlink ref="I16" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000025000000}"/>
+    <hyperlink ref="G17" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0500-000026000000}"/>
+    <hyperlink ref="G18" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0500-000027000000}"/>
+    <hyperlink ref="G19" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0500-000028000000}"/>
+    <hyperlink ref="G20" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0500-000029000000}"/>
+    <hyperlink ref="H17" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0500-00002A000000}"/>
+    <hyperlink ref="H18" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0500-00002B000000}"/>
+    <hyperlink ref="H19" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0500-00002C000000}"/>
+    <hyperlink ref="H20" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0500-00002D000000}"/>
+    <hyperlink ref="I17" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-00002E000000}"/>
+    <hyperlink ref="I18" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-00002F000000}"/>
+    <hyperlink ref="I19" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000030000000}"/>
+    <hyperlink ref="I20" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000031000000}"/>
+    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0500-000032000000}"/>
+    <hyperlink ref="H21" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0500-000033000000}"/>
+    <hyperlink ref="I21" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000034000000}"/>
+    <hyperlink ref="G27" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0500-000035000000}"/>
+    <hyperlink ref="H27" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0500-000036000000}"/>
+    <hyperlink ref="L27" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000037000000}"/>
+    <hyperlink ref="N27" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0500-000038000000}"/>
+    <hyperlink ref="G24" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0500-000039000000}"/>
+    <hyperlink ref="G25" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0500-00003A000000}"/>
+    <hyperlink ref="G22" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0500-00003B000000}"/>
+    <hyperlink ref="G23" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0500-00003C000000}"/>
+    <hyperlink ref="G26" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0500-00003D000000}"/>
+    <hyperlink ref="I10:I15" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0500-00003E000000}"/>
+    <hyperlink ref="J17:J21" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0500-00003F000000}"/>
+    <hyperlink ref="J16" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0500-000040000000}"/>
+    <hyperlink ref="I27" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0500-000041000000}"/>
+    <hyperlink ref="J27" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0500-000042000000}"/>
+    <hyperlink ref="M27" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0500-000043000000}"/>
+    <hyperlink ref="K27" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0500-000044000000}"/>
+    <hyperlink ref="O27" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0500-000045000000}"/>
+    <hyperlink ref="G28" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0500-000046000000}"/>
+    <hyperlink ref="G30" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0500-000047000000}"/>
+    <hyperlink ref="H28" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0500-000048000000}"/>
+    <hyperlink ref="H30" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0500-000049000000}"/>
+    <hyperlink ref="L28" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-00004A000000}"/>
+    <hyperlink ref="L30" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-00004B000000}"/>
+    <hyperlink ref="N28" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0500-00004C000000}"/>
+    <hyperlink ref="N30" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0500-00004D000000}"/>
+    <hyperlink ref="I28" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0500-00004E000000}"/>
+    <hyperlink ref="I30" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0500-00004F000000}"/>
+    <hyperlink ref="J28" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0500-000050000000}"/>
+    <hyperlink ref="J30" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0500-000051000000}"/>
+    <hyperlink ref="M28" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0500-000052000000}"/>
+    <hyperlink ref="M30" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0500-000053000000}"/>
+    <hyperlink ref="K28" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0500-000054000000}"/>
+    <hyperlink ref="K30" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0500-000055000000}"/>
+    <hyperlink ref="O28" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0500-000056000000}"/>
+    <hyperlink ref="O30" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0500-000057000000}"/>
+    <hyperlink ref="G31" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0500-000058000000}"/>
+    <hyperlink ref="H31" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0500-000059000000}"/>
+    <hyperlink ref="K31" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-00005A000000}"/>
+    <hyperlink ref="M31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0500-00005B000000}"/>
+    <hyperlink ref="I31" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0500-00005C000000}"/>
+    <hyperlink ref="L31" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0500-00005D000000}"/>
+    <hyperlink ref="J31" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0500-00005E000000}"/>
+    <hyperlink ref="N31" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0500-00005F000000}"/>
+    <hyperlink ref="G29" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0500-000060000000}"/>
+    <hyperlink ref="H29" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0500-000061000000}"/>
+    <hyperlink ref="L29" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000062000000}"/>
+    <hyperlink ref="N29" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0500-000063000000}"/>
+    <hyperlink ref="I29" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0500-000064000000}"/>
+    <hyperlink ref="J29" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0500-000065000000}"/>
+    <hyperlink ref="M29" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0500-000066000000}"/>
+    <hyperlink ref="K29" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0500-000067000000}"/>
+    <hyperlink ref="O29" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0500-000068000000}"/>
+    <hyperlink ref="G32" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0500-000069000000}"/>
+    <hyperlink ref="H32" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0500-00006A000000}"/>
+    <hyperlink ref="L32" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-00006B000000}"/>
+    <hyperlink ref="N32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0500-00006C000000}"/>
+    <hyperlink ref="I32" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0500-00006D000000}"/>
+    <hyperlink ref="J32" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0500-00006E000000}"/>
+    <hyperlink ref="M32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0500-00006F000000}"/>
+    <hyperlink ref="O32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0500-000070000000}"/>
+    <hyperlink ref="P32" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0500-000071000000}"/>
+    <hyperlink ref="G34" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0500-000072000000}"/>
+    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0500-000073000000}"/>
+    <hyperlink ref="H37" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0500-000074000000}"/>
+    <hyperlink ref="H33" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0500-000075000000}"/>
+    <hyperlink ref="I33" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0500-000076000000}"/>
+    <hyperlink ref="J33" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0500-000077000000}"/>
+    <hyperlink ref="K33" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000078000000}"/>
+    <hyperlink ref="L33" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0500-000079000000}"/>
+    <hyperlink ref="M33" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0500-00007A000000}"/>
+    <hyperlink ref="N33" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0500-00007B000000}"/>
+    <hyperlink ref="G33" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{00000000-0004-0000-0500-00007C000000}"/>
+    <hyperlink ref="H34" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{00000000-0004-0000-0500-00007D000000}"/>
+    <hyperlink ref="J34" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0500-00007E000000}"/>
+    <hyperlink ref="K34" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0500-00007F000000}"/>
+    <hyperlink ref="L34" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000080000000}"/>
+    <hyperlink ref="M34" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0500-000081000000}"/>
+    <hyperlink ref="N34" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0500-000082000000}"/>
+    <hyperlink ref="O34" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0500-000083000000}"/>
+    <hyperlink ref="M35" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0500-000084000000}"/>
+    <hyperlink ref="G38" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000085000000}"/>
+    <hyperlink ref="G39" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0500-000086000000}"/>
+    <hyperlink ref="H38" location="'giftCardReport++'!A1" display="giftCardReport" xr:uid="{00000000-0004-0000-0500-000087000000}"/>
+    <hyperlink ref="H39" location="'giftCardReport++'!A1" display="giftCardReport" xr:uid="{00000000-0004-0000-0500-000088000000}"/>
+    <hyperlink ref="K32" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0500-000089000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -11064,11 +11823,127 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E073C6-B7C5-4623-9530-E2A3BA724409}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="24" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="24" customHeight="1">
+      <c r="A1" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>362</v>
+      </c>
+      <c r="E1" s="62" t="s">
+        <v>363</v>
+      </c>
+      <c r="F1" s="62" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="24" customHeight="1">
+      <c r="A2" s="19">
+        <v>42</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>355</v>
+      </c>
+      <c r="C2" s="33">
+        <v>1</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>365</v>
+      </c>
+      <c r="E2" s="33">
+        <v>240</v>
+      </c>
+      <c r="F2" s="33">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABBCE883-5417-49C3-A23E-3201419BA613}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="31.5" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="31.5" customHeight="1">
+      <c r="A1" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="31.5" customHeight="1">
+      <c r="A2" s="19">
+        <v>42</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>355</v>
+      </c>
+      <c r="C2" s="33">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{04EF977E-89A6-47AE-9992-250C449FFE72}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:I16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11557,635 +12432,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="33.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30">
-      <c r="A2" s="19">
-        <v>26</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>313</v>
-      </c>
-      <c r="C2" s="20">
-        <v>1</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="45">
-      <c r="A3" s="19">
-        <v>27</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>329</v>
-      </c>
-      <c r="C3" s="20">
-        <v>1</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="45">
-      <c r="A4" s="19">
-        <v>28</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>330</v>
-      </c>
-      <c r="C4" s="20">
-        <v>1</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30">
-      <c r="A5" s="19">
-        <v>29</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>314</v>
-      </c>
-      <c r="C5" s="20">
-        <v>1</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30">
-      <c r="A6" s="19">
-        <v>30</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="C6" s="20">
-        <v>1</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30">
-      <c r="A7" s="20">
-        <v>31</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="C7" s="20">
-        <v>1</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="20">
-        <v>32</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>334</v>
-      </c>
-      <c r="C8" s="20">
-        <v>1</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="42">
-        <v>33</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="C9" s="20">
-        <v>1</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="42">
-        <v>34</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>336</v>
-      </c>
-      <c r="C10" s="20">
-        <v>1</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="42">
-        <v>35</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="C11" s="43">
-        <v>1</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="42">
-        <v>36</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="C12" s="43">
-        <v>1</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>325</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
-      <formula1>"payUcreditcard,Cash_Deposits"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1">
-      <c r="A1" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="30">
-      <c r="A2" s="19">
-        <v>26</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>313</v>
-      </c>
-      <c r="C2" s="30">
-        <v>1</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="30">
-        <v>2000</v>
-      </c>
-      <c r="L2" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="M2" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="N2" s="32" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" ht="45">
-      <c r="A3" s="19">
-        <v>27</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>329</v>
-      </c>
-      <c r="C3" s="30">
-        <v>1</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="I3" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="K3" s="30">
-        <v>2000</v>
-      </c>
-      <c r="L3" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="N3" s="32" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="5" customFormat="1" ht="45">
-      <c r="A4" s="19">
-        <v>28</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>330</v>
-      </c>
-      <c r="C4" s="30">
-        <v>1</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="J4" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="K4" s="30">
-        <v>2000</v>
-      </c>
-      <c r="L4" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="M4" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="N4" s="32" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="5" customFormat="1" ht="30">
-      <c r="A5" s="19">
-        <v>29</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>314</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="J5" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" s="30">
-        <v>2000</v>
-      </c>
-      <c r="L5" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="M5" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="N5" s="32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="5" customFormat="1" ht="30">
-      <c r="A6" s="19">
-        <v>30</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>315</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="J6" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="K6" s="30">
-        <v>2000</v>
-      </c>
-      <c r="L6" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="M6" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="N6" s="32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="5" customFormat="1" ht="30">
-      <c r="A7" s="19">
-        <v>31</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="H7" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="I7" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="J7" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="K7" s="30">
-        <v>2000</v>
-      </c>
-      <c r="L7" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="M7" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="N7" s="32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="5" customFormat="1" ht="30">
-      <c r="A8" s="19">
-        <v>32</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>334</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="G8" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="I8" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="J8" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="K8" s="30">
-        <v>2000</v>
-      </c>
-      <c r="L8" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="M8" s="31" t="s">
-        <v>189</v>
-      </c>
-      <c r="N8" s="32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="30">
-      <c r="A9" s="42">
-        <v>35</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="I9" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="J9" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="K9" s="30">
-        <v>2000</v>
-      </c>
-      <c r="L9" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="M9" s="31" t="s">
-        <v>189</v>
-      </c>
-      <c r="N9" s="32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1"/>
-    <hyperlink ref="M3" r:id="rId2"/>
-    <hyperlink ref="M4" r:id="rId3"/>
-    <hyperlink ref="M5" r:id="rId4"/>
-    <hyperlink ref="M8" r:id="rId5"/>
-    <hyperlink ref="M6" r:id="rId6"/>
-    <hyperlink ref="M7" r:id="rId7"/>
-    <hyperlink ref="M9" r:id="rId8"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
TA245 51 Test case - clear whishlist by default. 52 Test case - clear whishlist by adding a product.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup.xlsx
+++ b/src/test/resources/data/jdgroup.xlsx
@@ -1,58 +1,65 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34642\git\TA245\JD_IC_TestAutomationTA245\src\test\resources\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645109BF-92DF-4328-9826-4F0D3AFF5609}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="IC_ProductsSortBy++" sheetId="39" r:id="rId1"/>
-    <sheet name="ic_SubscribeNews_DupliEmailID++" sheetId="38" r:id="rId2"/>
-    <sheet name="IC" sheetId="32" r:id="rId3"/>
-    <sheet name="EnterBasicDetails++" sheetId="33" r:id="rId4"/>
-    <sheet name="EnterSpouseInfor++" sheetId="34" r:id="rId5"/>
-    <sheet name="EnterContact++" sheetId="35" r:id="rId6"/>
-    <sheet name="CreditEnterAddressDetails++" sheetId="36" r:id="rId7"/>
-    <sheet name="CreditEnterEmploymentDetails++" sheetId="37" r:id="rId8"/>
-    <sheet name="CreditStatusVerification++" sheetId="1" r:id="rId9"/>
-    <sheet name="CreditApp_NavigateFilter++" sheetId="2" r:id="rId10"/>
-    <sheet name="giftCardReport++" sheetId="3" r:id="rId11"/>
-    <sheet name="adminUserUpdate++" sheetId="4" r:id="rId12"/>
-    <sheet name="ICUpdateUser++" sheetId="5" r:id="rId13"/>
-    <sheet name="SapCustomer++" sheetId="6" r:id="rId14"/>
-    <sheet name="Suites" sheetId="7" r:id="rId15"/>
-    <sheet name="PayUPagePayment++" sheetId="8" r:id="rId16"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="9" r:id="rId17"/>
-    <sheet name="deliveryPopulation++" sheetId="10" r:id="rId18"/>
-    <sheet name="icGiftCardPurchase++" sheetId="11" r:id="rId19"/>
-    <sheet name="SAP_OrderRelated++" sheetId="12" r:id="rId20"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="13" r:id="rId21"/>
-    <sheet name="OrderStatusSearch++" sheetId="14" r:id="rId22"/>
-    <sheet name="Login_magento++" sheetId="15" r:id="rId23"/>
-    <sheet name="ic_RetriveOrderID++" sheetId="16" r:id="rId24"/>
-    <sheet name="ProductSearch++" sheetId="17" r:id="rId25"/>
-    <sheet name="icRedeemGiftCard++" sheetId="18" r:id="rId26"/>
-    <sheet name="VeriyGiftcardUsableity++" sheetId="19" r:id="rId27"/>
-    <sheet name="ic_login++" sheetId="20" r:id="rId28"/>
-    <sheet name="DB_connection_master++" sheetId="21" r:id="rId29"/>
-    <sheet name="icGiftCardVerificationSender++" sheetId="22" r:id="rId30"/>
-    <sheet name="ic_CashDepositPayment++" sheetId="23" r:id="rId31"/>
-    <sheet name="CreateaccountBackend++" sheetId="24" r:id="rId32"/>
-    <sheet name="accountCreation++" sheetId="25" r:id="rId33"/>
-    <sheet name="Russels" sheetId="26" r:id="rId34"/>
-    <sheet name="Login++" sheetId="27" r:id="rId35"/>
-    <sheet name="Bradlows" sheetId="28" r:id="rId36"/>
-    <sheet name="Rochester" sheetId="29" r:id="rId37"/>
-    <sheet name="Sleepmasters" sheetId="30" r:id="rId38"/>
-    <sheet name="HiFiCorp" sheetId="31" r:id="rId39"/>
+    <sheet name="IC" sheetId="32" r:id="rId1"/>
+    <sheet name="ic_NavigetoWishlist++" sheetId="40" r:id="rId2"/>
+    <sheet name="IC_ProductsSortBy++" sheetId="39" r:id="rId3"/>
+    <sheet name="ic_SubscribeNews_DupliEmailID++" sheetId="38" r:id="rId4"/>
+    <sheet name="EnterBasicDetails++" sheetId="33" r:id="rId5"/>
+    <sheet name="EnterSpouseInfor++" sheetId="34" r:id="rId6"/>
+    <sheet name="EnterContact++" sheetId="35" r:id="rId7"/>
+    <sheet name="CreditEnterAddressDetails++" sheetId="36" r:id="rId8"/>
+    <sheet name="CreditEnterEmploymentDetails++" sheetId="37" r:id="rId9"/>
+    <sheet name="CreditStatusVerification++" sheetId="1" r:id="rId10"/>
+    <sheet name="CreditApp_NavigateFilter++" sheetId="2" r:id="rId11"/>
+    <sheet name="giftCardReport++" sheetId="3" r:id="rId12"/>
+    <sheet name="adminUserUpdate++" sheetId="4" r:id="rId13"/>
+    <sheet name="ICUpdateUser++" sheetId="5" r:id="rId14"/>
+    <sheet name="SapCustomer++" sheetId="6" r:id="rId15"/>
+    <sheet name="Suites" sheetId="7" r:id="rId16"/>
+    <sheet name="PayUPagePayment++" sheetId="8" r:id="rId17"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="9" r:id="rId18"/>
+    <sheet name="deliveryPopulation++" sheetId="10" r:id="rId19"/>
+    <sheet name="icGiftCardPurchase++" sheetId="11" r:id="rId20"/>
+    <sheet name="SAP_OrderRelated++" sheetId="12" r:id="rId21"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="13" r:id="rId22"/>
+    <sheet name="OrderStatusSearch++" sheetId="14" r:id="rId23"/>
+    <sheet name="Login_magento++" sheetId="15" r:id="rId24"/>
+    <sheet name="ic_RetriveOrderID++" sheetId="16" r:id="rId25"/>
+    <sheet name="ProductSearch++" sheetId="17" r:id="rId26"/>
+    <sheet name="icRedeemGiftCard++" sheetId="18" r:id="rId27"/>
+    <sheet name="VeriyGiftcardUsableity++" sheetId="19" r:id="rId28"/>
+    <sheet name="ic_login++" sheetId="20" r:id="rId29"/>
+    <sheet name="DB_connection_master++" sheetId="21" r:id="rId30"/>
+    <sheet name="icGiftCardVerificationSender++" sheetId="22" r:id="rId31"/>
+    <sheet name="ic_CashDepositPayment++" sheetId="23" r:id="rId32"/>
+    <sheet name="CreateaccountBackend++" sheetId="24" r:id="rId33"/>
+    <sheet name="accountCreation++" sheetId="25" r:id="rId34"/>
+    <sheet name="Russels" sheetId="26" r:id="rId35"/>
+    <sheet name="Login++" sheetId="27" r:id="rId36"/>
+    <sheet name="Bradlows" sheetId="28" r:id="rId37"/>
+    <sheet name="Rochester" sheetId="29" r:id="rId38"/>
+    <sheet name="Sleepmasters" sheetId="30" r:id="rId39"/>
+    <sheet name="HiFiCorp" sheetId="31" r:id="rId40"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3709" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3723" uniqueCount="537">
   <si>
     <t>TCID</t>
   </si>
@@ -1642,16 +1649,44 @@
   </si>
   <si>
     <t>Registered customer from sales order</t>
+  </si>
+  <si>
+    <t>Wish List - Clear Wish List</t>
+  </si>
+  <si>
+    <t>ic_NavigetoWishlist</t>
+  </si>
+  <si>
+    <t>Login_type</t>
+  </si>
+  <si>
+    <t>ExistingUser</t>
+  </si>
+  <si>
+    <t>TimeOut_seconds</t>
+  </si>
+  <si>
+    <t>Praveen.Ojha@itcinfotech.com</t>
+  </si>
+  <si>
+    <t>Test123#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1804,79 +1839,82 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -1935,6 +1973,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1982,7 +2023,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2015,9 +2056,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2050,6 +2108,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2225,74 +2300,1600 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Q47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="3" customFormat="1">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="3" customFormat="1">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="3" customFormat="1">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="3" customFormat="1">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="3" customFormat="1">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="3" customFormat="1">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="3" customFormat="1">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="3">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="3">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="3">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="3">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="3">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="3">
+        <v>17</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="3">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="3">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="3">
+        <v>20</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="3">
+        <v>21</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="9">
+        <v>9</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="8">
+        <v>15</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="9">
+        <v>17</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="9">
+        <v>18</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="12">
+        <v>16</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="12">
+        <v>17</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="12">
+        <v>18</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="12">
+        <v>19</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="9">
+        <v>16</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+    </row>
+    <row r="29" spans="1:16" s="3" customFormat="1">
+      <c r="A29" s="3">
+        <v>2</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="9">
+        <v>14</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="2">
+        <v>1</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>404</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13" t="s">
+        <v>404</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="N31" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="O31" s="8" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="2">
+        <v>42</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="I32" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="17"/>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" s="9">
+        <v>40</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34" s="9">
+        <v>41</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35" s="3">
+        <v>42</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36" s="20">
+        <v>43</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>414</v>
+      </c>
+      <c r="C36" s="2">
+        <v>181</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>414</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" s="25" customFormat="1">
+      <c r="A37" s="24">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
+        <v>496</v>
+      </c>
+      <c r="C37" s="25">
+        <v>195</v>
+      </c>
+      <c r="D37" t="s">
+        <v>416</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" s="25" customFormat="1">
+      <c r="A38" s="24">
+        <v>45</v>
+      </c>
+      <c r="B38" t="s">
+        <v>497</v>
+      </c>
+      <c r="C38" s="25">
+        <v>196</v>
+      </c>
+      <c r="D38" t="s">
+        <v>418</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" s="25" customFormat="1">
+      <c r="A39" s="27">
+        <v>46</v>
+      </c>
+      <c r="B39" s="28" t="s">
+        <v>503</v>
+      </c>
+      <c r="C39" s="29">
+        <v>203</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>503</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" t="s">
+        <v>372</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="30"/>
+      <c r="P39" s="27"/>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40" t="s">
+        <v>152</v>
+      </c>
+      <c r="B40" t="s">
+        <v>510</v>
+      </c>
+      <c r="C40" s="2">
+        <v>215</v>
+      </c>
+      <c r="D40" t="s">
+        <v>510</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" t="s">
+        <v>511</v>
+      </c>
+      <c r="C41" s="2">
+        <v>216</v>
+      </c>
+      <c r="D41" t="s">
+        <v>511</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G41" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="A42" t="s">
+        <v>156</v>
+      </c>
+      <c r="B42" t="s">
+        <v>512</v>
+      </c>
+      <c r="C42" s="2">
+        <v>217</v>
+      </c>
+      <c r="D42" t="s">
+        <v>512</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43">
+        <v>47</v>
+      </c>
+      <c r="B43" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" t="s">
+        <v>114</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G43" t="s">
+        <v>377</v>
+      </c>
+      <c r="H43" t="s">
+        <v>379</v>
+      </c>
+      <c r="I43" t="s">
+        <v>380</v>
+      </c>
+      <c r="J43" t="s">
+        <v>386</v>
+      </c>
+      <c r="K43" t="s">
+        <v>364</v>
+      </c>
+      <c r="L43" t="s">
+        <v>387</v>
+      </c>
+      <c r="M43" t="s">
+        <v>382</v>
+      </c>
+      <c r="N43" t="s">
+        <v>365</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="P43" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="A44">
+        <v>48</v>
+      </c>
+      <c r="B44" t="s">
+        <v>515</v>
+      </c>
+      <c r="D44" t="s">
+        <v>515</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="H44" t="s">
+        <v>377</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="N44" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="P44" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q44" s="4" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="A45">
+        <v>49</v>
+      </c>
+      <c r="B45" t="s">
+        <v>516</v>
+      </c>
+      <c r="D45" t="s">
+        <v>516</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="I45" t="s">
+        <v>379</v>
+      </c>
+      <c r="J45" t="s">
+        <v>380</v>
+      </c>
+      <c r="K45" t="s">
+        <v>386</v>
+      </c>
+      <c r="L45" t="s">
+        <v>364</v>
+      </c>
+      <c r="M45" t="s">
+        <v>387</v>
+      </c>
+      <c r="N45" t="s">
+        <v>382</v>
+      </c>
+      <c r="O45" t="s">
+        <v>518</v>
+      </c>
+      <c r="P45" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
+      <c r="A46">
+        <v>50</v>
+      </c>
+      <c r="B46" t="s">
+        <v>517</v>
+      </c>
+      <c r="D46" t="s">
+        <v>517</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="H46" t="s">
+        <v>377</v>
+      </c>
+      <c r="I46" t="s">
+        <v>379</v>
+      </c>
+      <c r="J46" t="s">
+        <v>380</v>
+      </c>
+      <c r="K46" t="s">
+        <v>386</v>
+      </c>
+      <c r="L46" t="s">
+        <v>364</v>
+      </c>
+      <c r="M46" t="s">
+        <v>387</v>
+      </c>
+      <c r="N46" t="s">
+        <v>382</v>
+      </c>
+      <c r="O46" t="s">
+        <v>518</v>
+      </c>
+      <c r="P46" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="A47" s="2">
+        <v>51</v>
+      </c>
+      <c r="B47" s="32" t="s">
+        <v>530</v>
+      </c>
+      <c r="D47" s="32" t="s">
+        <v>530</v>
+      </c>
+      <c r="E47" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="G47" s="32" t="s">
+        <v>531</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="G29" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="G22:G23" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="H22" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="H23" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="G31" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="I31" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="L31" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="N31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="H2" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="J2" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="G2" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="J3" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="G3" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="H4" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="J4" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="G4" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="H5" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="J5" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="G5" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="H6" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="J6" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="G6" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="I8:I9" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="I7" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="H37" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="H38" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="I37" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="I38" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="J37" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="J38" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="K37" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="K38" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="L37" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="L38" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="G38" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="G39" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="O43" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="P45" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="I44" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="G44" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
+    <hyperlink ref="H45" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
+    <hyperlink ref="J44" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
+    <hyperlink ref="K44" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
+    <hyperlink ref="L44" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
+    <hyperlink ref="M44" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0200-000033000000}"/>
+    <hyperlink ref="N44" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0200-000034000000}"/>
+    <hyperlink ref="O44" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0200-000035000000}"/>
+    <hyperlink ref="Q44" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-000036000000}"/>
+    <hyperlink ref="G45:G46" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0200-000037000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="22"/>
-    <col min="2" max="2" width="10" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="22"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>505</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>509</v>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2300,8 +3901,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2341,8 +3942,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2514,8 +4115,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3129,8 +4730,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5367,11 +6968,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -5832,8 +7433,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6006,8 +7607,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6661,8 +8262,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6900,8 +8501,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7564,8 +9165,78 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A66950F7-A2A2-46EE-A864-6D5B94E933C4}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>532</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="22">
+        <v>51</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>533</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>536</v>
+      </c>
+      <c r="F2">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{347D1B61-D266-4B4C-A4A7-7AE26E1A7C6D}">
+      <formula1>"ExistingUser,logedOn_user"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{26713E1D-5C00-4F62-9CD0-6C321063EC65}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7787,60 +9458,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="3" width="9.140625" style="22"/>
-    <col min="4" max="4" width="15.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="22"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>500</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="22">
-        <v>46</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>501</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>502</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8117,8 +9736,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8410,8 +10029,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8731,8 +10350,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -9375,8 +10994,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9612,8 +11231,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -10320,8 +11939,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10418,8 +12037,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10491,8 +12110,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10785,8 +12404,86 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="2" max="2" width="10" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>505</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>509</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10913,1543 +12610,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q46"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L23" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O43" sqref="O43"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" s="3" customFormat="1">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" s="3" customFormat="1">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" s="3" customFormat="1">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="3" customFormat="1">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" s="3" customFormat="1">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>372</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" s="3" customFormat="1">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" s="3" customFormat="1">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="3">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="3">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="3">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="3">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="3">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="3">
-        <v>17</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="3">
-        <v>18</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-    </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="3">
-        <v>19</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-    </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="3">
-        <v>20</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="3">
-        <v>21</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-    </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="9">
-        <v>9</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16">
-      <c r="A21" s="8">
-        <v>15</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="7" t="s">
-        <v>384</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="M21" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-    </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="9">
-        <v>17</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>384</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="9">
-        <v>18</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>384</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="K23" s="11" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="12">
-        <v>16</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="12">
-        <v>17</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="12">
-        <v>18</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="A27" s="12">
-        <v>19</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-    </row>
-    <row r="28" spans="1:16">
-      <c r="A28" s="9">
-        <v>16</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-    </row>
-    <row r="29" spans="1:16" s="3" customFormat="1">
-      <c r="A29" s="3">
-        <v>2</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16">
-      <c r="A30" s="9">
-        <v>14</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-    </row>
-    <row r="31" spans="1:16">
-      <c r="A31" s="2">
-        <v>1</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>404</v>
-      </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13" t="s">
-        <v>404</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="N31" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="O31" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16">
-      <c r="A32" s="2">
-        <v>42</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17" t="s">
-        <v>364</v>
-      </c>
-      <c r="H32" s="17" t="s">
-        <v>406</v>
-      </c>
-      <c r="I32" s="17" t="s">
-        <v>407</v>
-      </c>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="17"/>
-    </row>
-    <row r="33" spans="1:17">
-      <c r="A33" s="9">
-        <v>40</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17">
-      <c r="A34" s="9">
-        <v>41</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17">
-      <c r="A35" s="3">
-        <v>42</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17">
-      <c r="A36" s="20">
-        <v>43</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>414</v>
-      </c>
-      <c r="C36" s="2">
-        <v>181</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>414</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" s="25" customFormat="1">
-      <c r="A37" s="24">
-        <v>44</v>
-      </c>
-      <c r="B37" t="s">
-        <v>496</v>
-      </c>
-      <c r="C37" s="25">
-        <v>195</v>
-      </c>
-      <c r="D37" t="s">
-        <v>416</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>494</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="L37" s="4" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" s="25" customFormat="1">
-      <c r="A38" s="24">
-        <v>45</v>
-      </c>
-      <c r="B38" t="s">
-        <v>497</v>
-      </c>
-      <c r="C38" s="25">
-        <v>196</v>
-      </c>
-      <c r="D38" t="s">
-        <v>418</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>494</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="L38" s="4" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" s="25" customFormat="1">
-      <c r="A39" s="27">
-        <v>46</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>503</v>
-      </c>
-      <c r="C39" s="29">
-        <v>203</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>503</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F39" t="s">
-        <v>372</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>504</v>
-      </c>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="19"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="27"/>
-    </row>
-    <row r="40" spans="1:17">
-      <c r="A40" t="s">
-        <v>152</v>
-      </c>
-      <c r="B40" t="s">
-        <v>510</v>
-      </c>
-      <c r="C40" s="2">
-        <v>215</v>
-      </c>
-      <c r="D40" t="s">
-        <v>510</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G40" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17">
-      <c r="A41" t="s">
-        <v>154</v>
-      </c>
-      <c r="B41" t="s">
-        <v>511</v>
-      </c>
-      <c r="C41" s="2">
-        <v>216</v>
-      </c>
-      <c r="D41" t="s">
-        <v>511</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G41" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17">
-      <c r="A42" t="s">
-        <v>156</v>
-      </c>
-      <c r="B42" t="s">
-        <v>512</v>
-      </c>
-      <c r="C42" s="2">
-        <v>217</v>
-      </c>
-      <c r="D42" t="s">
-        <v>512</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G42" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17">
-      <c r="A43">
-        <v>47</v>
-      </c>
-      <c r="B43" t="s">
-        <v>114</v>
-      </c>
-      <c r="D43" t="s">
-        <v>114</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G43" t="s">
-        <v>377</v>
-      </c>
-      <c r="H43" t="s">
-        <v>379</v>
-      </c>
-      <c r="I43" t="s">
-        <v>380</v>
-      </c>
-      <c r="J43" t="s">
-        <v>386</v>
-      </c>
-      <c r="K43" t="s">
-        <v>364</v>
-      </c>
-      <c r="L43" t="s">
-        <v>387</v>
-      </c>
-      <c r="M43" t="s">
-        <v>382</v>
-      </c>
-      <c r="N43" t="s">
-        <v>365</v>
-      </c>
-      <c r="O43" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="P43" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17">
-      <c r="A44">
-        <v>48</v>
-      </c>
-      <c r="B44" t="s">
-        <v>515</v>
-      </c>
-      <c r="D44" t="s">
-        <v>515</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="H44" t="s">
-        <v>377</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="L44" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="M44" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="N44" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="O44" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="P44" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q44" s="4" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17">
-      <c r="A45">
-        <v>49</v>
-      </c>
-      <c r="B45" t="s">
-        <v>516</v>
-      </c>
-      <c r="D45" t="s">
-        <v>516</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="I45" t="s">
-        <v>379</v>
-      </c>
-      <c r="J45" t="s">
-        <v>380</v>
-      </c>
-      <c r="K45" t="s">
-        <v>386</v>
-      </c>
-      <c r="L45" t="s">
-        <v>364</v>
-      </c>
-      <c r="M45" t="s">
-        <v>387</v>
-      </c>
-      <c r="N45" t="s">
-        <v>382</v>
-      </c>
-      <c r="O45" t="s">
-        <v>518</v>
-      </c>
-      <c r="P45" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17">
-      <c r="A46">
-        <v>50</v>
-      </c>
-      <c r="B46" t="s">
-        <v>517</v>
-      </c>
-      <c r="D46" t="s">
-        <v>517</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="H46" t="s">
-        <v>377</v>
-      </c>
-      <c r="I46" t="s">
-        <v>379</v>
-      </c>
-      <c r="J46" t="s">
-        <v>380</v>
-      </c>
-      <c r="K46" t="s">
-        <v>386</v>
-      </c>
-      <c r="L46" t="s">
-        <v>364</v>
-      </c>
-      <c r="M46" t="s">
-        <v>387</v>
-      </c>
-      <c r="N46" t="s">
-        <v>382</v>
-      </c>
-      <c r="O46" t="s">
-        <v>518</v>
-      </c>
-      <c r="P46" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>366</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="G29" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G22:G23" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="H22" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H23" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="G31" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="I31" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="L31" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="N31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="H2" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="J2" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G2" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="J3" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G3" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="H4" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="J4" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G4" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="H5" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="J5" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G5" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="H6" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="J6" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G6" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
-    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
-    <hyperlink ref="I8:I9" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="I7" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="H37" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
-    <hyperlink ref="H38" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
-    <hyperlink ref="I37" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
-    <hyperlink ref="I38" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
-    <hyperlink ref="J37" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
-    <hyperlink ref="J38" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
-    <hyperlink ref="K37" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
-    <hyperlink ref="K38" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
-    <hyperlink ref="L37" location="'EnterContact++'!A1" display="EnterContact"/>
-    <hyperlink ref="L38" location="'EnterContact++'!A1" display="EnterContact"/>
-    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G38" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G39" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID"/>
-    <hyperlink ref="O43" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="P45" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
-    <hyperlink ref="I44" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="G44" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="H45" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="J44" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="K44" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="L44" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="M44" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="N44" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="O44" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
-    <hyperlink ref="Q44" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G45:G46" location="'ic_login++'!A1" display="ic_login"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12566,8 +12728,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12607,8 +12769,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13114,8 +13276,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13776,8 +13938,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13921,8 +14083,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -14116,8 +14278,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -14252,8 +14414,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -14388,8 +14550,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -14524,8 +14686,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="22"/>
+    <col min="4" max="4" width="15.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>500</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="22">
+        <v>46</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>501</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>502</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -14660,8 +14874,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -14895,8 +15109,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15039,8 +15253,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15143,8 +15357,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15267,8 +15481,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15383,57 +15597,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>